<commit_message>
added ladder network results to performance file
</commit_message>
<xml_diff>
--- a/summary/performances.xlsx
+++ b/summary/performances.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucan\OneDrive - Politecnico di Milano\PhD\progetti\CIBB2018\summary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/canakoglu/GMQL-sources/CIBB2018/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A3BD19-F42A-4E9C-B133-54069D6C8362}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{669412F2-50BC-C24E-8080-76EC5D061859}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCGA_info" sheetId="3" r:id="rId1"/>
     <sheet name="TL" sheetId="1" r:id="rId2"/>
     <sheet name="DM" sheetId="2" r:id="rId3"/>
+    <sheet name="LADDER" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="57">
   <si>
     <t>accuracy</t>
   </si>
@@ -178,13 +179,28 @@
   </si>
   <si>
     <t>For this matrix I used only the top 5000 variant genes and their 5 neighbors ( = 25000 features)</t>
+  </si>
+  <si>
+    <t>LADDER NETWORK</t>
+  </si>
+  <si>
+    <t>KIDNEY</t>
+  </si>
+  <si>
+    <t>LUNG</t>
+  </si>
+  <si>
+    <t>In this implementation, as we agreed with Luca, I have done upsampling on the healthy cases. In other words, we replicated the healthy samples as many as needed to reach the same name of the tumorious cases.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Without upsampling, it was working better. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,16 +255,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -289,11 +318,156 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -305,6 +479,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -324,15 +507,34 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -350,7 +552,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -431,7 +633,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1116,7 +1318,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="460990440"/>
@@ -1175,7 +1377,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="460991752"/>
@@ -1217,7 +1419,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1247,7 +1449,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1843,7 +2045,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2166,21 +2368,21 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D4" sqref="A4:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -2197,7 +2399,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2214,7 +2416,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -2231,7 +2433,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -2248,7 +2450,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -2265,7 +2467,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2282,7 +2484,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -2299,7 +2501,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2316,7 +2518,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -2333,7 +2535,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2350,7 +2552,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -2367,7 +2569,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -2384,7 +2586,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -2401,7 +2603,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
@@ -2418,7 +2620,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -2435,7 +2637,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -2452,7 +2654,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -2469,7 +2671,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -2486,7 +2688,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -2503,7 +2705,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -2520,7 +2722,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
@@ -2537,7 +2739,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
@@ -2554,7 +2756,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
@@ -2571,7 +2773,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>36</v>
       </c>
@@ -2588,7 +2790,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>12</v>
       </c>
@@ -2605,7 +2807,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -2622,7 +2824,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
@@ -2639,7 +2841,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
@@ -2656,7 +2858,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>40</v>
       </c>
@@ -2673,7 +2875,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
@@ -2690,7 +2892,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
@@ -2707,7 +2909,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
@@ -2724,7 +2926,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
@@ -2741,7 +2943,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>44</v>
       </c>
@@ -2772,35 +2974,35 @@
   <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:23" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="G1" s="8" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="G1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="M1" s="8" t="s">
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="M1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2837,15 +3039,15 @@
       <c r="Q2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="10" t="s">
+      <c r="S2" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2892,7 +3094,7 @@
         <v>0.8727243452125375</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2939,7 +3141,7 @@
         <v>0.94075163398692807</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -2986,7 +3188,7 @@
         <v>0.92877816627816634</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -3033,7 +3235,7 @@
         <v>0.93029331779331792</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -3080,7 +3282,7 @@
         <v>0.92328224377020118</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -3127,7 +3329,7 @@
         <v>0.90674048174048172</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -3174,7 +3376,7 @@
         <v>0.92949640287769797</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -3221,7 +3423,7 @@
         <v>0.92057008192122092</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -3268,7 +3470,7 @@
         <v>0.95059434621915884</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -3315,7 +3517,7 @@
         <v>0.93925925925925924</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -3362,7 +3564,7 @@
         <v>0.93595744680851067</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -3409,7 +3611,7 @@
         <v>0.93129770992366423</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -3456,7 +3658,7 @@
         <v>0.96538314176245199</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -3503,7 +3705,7 @@
         <v>0.9207496352822353</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -3550,7 +3752,7 @@
         <v>0.87643363728470125</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -3597,7 +3799,7 @@
         <v>0.92742919389978229</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -3644,7 +3846,7 @@
         <v>0.93150739704118346</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -3691,7 +3893,7 @@
         <v>0.93585105257590173</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>4</v>
       </c>
@@ -3747,7 +3949,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -3806,7 +4008,7 @@
         <v>-3.0769230769230882E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
@@ -3865,7 +4067,7 @@
         <v>-1.1764705882352899E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -3924,7 +4126,7 @@
         <v>-2.222222222222214E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
@@ -4000,27 +4202,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDBC07E4-70E4-4EA6-BC7B-0A2447B840E5}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="33.6" x14ac:dyDescent="0.65">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:12" ht="34" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4034,7 +4236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -4050,15 +4252,15 @@
       <c r="E3">
         <v>0.97312299999999996</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
@@ -4075,7 +4277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>49</v>
       </c>
@@ -4092,25 +4294,25 @@
         <v>0.97692299999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:12" ht="33.6" x14ac:dyDescent="0.65">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:12" ht="34" x14ac:dyDescent="0.4">
+      <c r="A9" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
         <v>0</v>
@@ -4124,16 +4326,16 @@
       <c r="E10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -4150,7 +4352,7 @@
         <v>0.98260899999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -4167,7 +4369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>49</v>
       </c>
@@ -4184,31 +4386,31 @@
         <v>0.99230799999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
     </row>
   </sheetData>
@@ -4220,4 +4422,656 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D156AB4A-B94F-484C-9210-CE1AAD538863}">
+  <dimension ref="B1:M25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:13" s="3" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="6"/>
+      <c r="I1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+    </row>
+    <row r="2" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="17"/>
+      <c r="C2" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B3" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="28">
+        <v>0.97701149425287304</v>
+      </c>
+      <c r="D3" s="28">
+        <v>0.890625</v>
+      </c>
+      <c r="E3" s="28">
+        <v>0.80281690140844997</v>
+      </c>
+      <c r="F3" s="29">
+        <v>1</v>
+      </c>
+      <c r="H3" s="22" t="str">
+        <f>VLOOKUP($B3,TL!$G3:$K20,1,FALSE)</f>
+        <v>BRCA</v>
+      </c>
+      <c r="I3" s="15">
+        <f>VLOOKUP($B3,TL!$G3:$K20,2,FALSE)</f>
+        <v>0.98851104186424599</v>
+      </c>
+      <c r="J3" s="15">
+        <f>VLOOKUP($B3,TL!$G3:$K20,3,FALSE)</f>
+        <v>0.94562199235649746</v>
+      </c>
+      <c r="K3" s="15">
+        <f>VLOOKUP($B3,TL!$G3:$K20,4,FALSE)</f>
+        <v>0.91041666666666676</v>
+      </c>
+      <c r="L3" s="15">
+        <f>VLOOKUP($B3,TL!$G3:$K20,5,FALSE)</f>
+        <v>0.9913043478260869</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B4" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="28">
+        <v>0.99019607843137203</v>
+      </c>
+      <c r="D4" s="28">
+        <v>0.96212121212121204</v>
+      </c>
+      <c r="E4" s="28">
+        <v>0.94074074074073999</v>
+      </c>
+      <c r="F4" s="29">
+        <v>0.98449612403100695</v>
+      </c>
+      <c r="H4" s="23" t="e">
+        <f>VLOOKUP($B4,TL!$G5:$K22,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I4" s="15" t="e">
+        <f>VLOOKUP($B4,TL!$G5:$K22,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J4" s="15" t="e">
+        <f>VLOOKUP($B4,TL!$G5:$K22,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K4" s="15" t="e">
+        <f>VLOOKUP($B4,TL!$G5:$K22,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L4" s="15" t="e">
+        <f>VLOOKUP($B4,TL!$G5:$K22,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B5" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="28">
+        <v>0.98317094774136404</v>
+      </c>
+      <c r="D5" s="28">
+        <v>0.92050209205020905</v>
+      </c>
+      <c r="E5" s="28">
+        <v>0.85271317829457305</v>
+      </c>
+      <c r="F5" s="29">
+        <v>1</v>
+      </c>
+      <c r="H5" s="23" t="e">
+        <f>VLOOKUP($B5,TL!$G6:$K23,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I5" s="15" t="e">
+        <f>VLOOKUP($B5,TL!$G6:$K23,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J5" s="15" t="e">
+        <f>VLOOKUP($B5,TL!$G6:$K23,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K5" s="15" t="e">
+        <f>VLOOKUP($B5,TL!$G6:$K23,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L5" s="15" t="e">
+        <f>VLOOKUP($B5,TL!$G6:$K23,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B6" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="28">
+        <v>0.960093896713615</v>
+      </c>
+      <c r="D6" s="28">
+        <v>0.679245283018868</v>
+      </c>
+      <c r="E6" s="28">
+        <v>0.52941176470588203</v>
+      </c>
+      <c r="F6" s="29">
+        <v>0.94736842105263097</v>
+      </c>
+      <c r="H6" s="23" t="str">
+        <f>VLOOKUP($B6,TL!$G4:$K21,1,FALSE)</f>
+        <v>BLCA</v>
+      </c>
+      <c r="I6" s="15">
+        <f>VLOOKUP($B6,TL!$G4:$K21,2,FALSE)</f>
+        <v>0.98823464269428707</v>
+      </c>
+      <c r="J6" s="15">
+        <f>VLOOKUP($B6,TL!$G4:$K21,3,FALSE)</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="K6" s="15">
+        <f>VLOOKUP($B6,TL!$G4:$K21,4,FALSE)</f>
+        <v>0.88333333333333319</v>
+      </c>
+      <c r="L6" s="15">
+        <f>VLOOKUP($B6,TL!$G4:$K21,5,FALSE)</f>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B7" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="28">
+        <v>0.94155844155844104</v>
+      </c>
+      <c r="D7" s="28">
+        <v>0</v>
+      </c>
+      <c r="E7" s="28">
+        <v>0</v>
+      </c>
+      <c r="F7" s="29">
+        <v>0</v>
+      </c>
+      <c r="H7" s="23" t="e">
+        <f>VLOOKUP($B7,TL!$G7:$K24,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I7" s="15" t="e">
+        <f>VLOOKUP($B7,TL!$G7:$K24,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J7" s="15" t="e">
+        <f>VLOOKUP($B7,TL!$G7:$K24,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K7" s="15" t="e">
+        <f>VLOOKUP($B7,TL!$G7:$K24,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L7" s="15" t="e">
+        <f>VLOOKUP($B7,TL!$G7:$K24,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B8" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="28">
+        <v>0.98480243161094205</v>
+      </c>
+      <c r="D8" s="28">
+        <v>0.94252873563218298</v>
+      </c>
+      <c r="E8" s="28">
+        <v>0.89130434782608603</v>
+      </c>
+      <c r="F8" s="29">
+        <v>1</v>
+      </c>
+      <c r="H8" s="23" t="str">
+        <f>VLOOKUP($B8,TL!$G8:$K25,1,FALSE)</f>
+        <v>COAD</v>
+      </c>
+      <c r="I8" s="15">
+        <f>VLOOKUP($B8,TL!$G8:$K25,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J8" s="15">
+        <f>VLOOKUP($B8,TL!$G8:$K25,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="K8" s="15">
+        <f>VLOOKUP($B8,TL!$G8:$K25,4,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="L8" s="15">
+        <f>VLOOKUP($B8,TL!$G8:$K25,5,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="28">
+        <v>0.96996466431095396</v>
+      </c>
+      <c r="D9" s="28">
+        <v>0.83168316831683098</v>
+      </c>
+      <c r="E9" s="28">
+        <v>0.73684210526315697</v>
+      </c>
+      <c r="F9" s="29">
+        <v>0.95454545454545403</v>
+      </c>
+      <c r="H9" s="23" t="e">
+        <f>VLOOKUP($B9,TL!$G9:$K26,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I9" s="15" t="e">
+        <f>VLOOKUP($B9,TL!$G9:$K26,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J9" s="15" t="e">
+        <f>VLOOKUP($B9,TL!$G9:$K26,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K9" s="15" t="e">
+        <f>VLOOKUP($B9,TL!$G9:$K26,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L9" s="15" t="e">
+        <f>VLOOKUP($B9,TL!$G9:$K26,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B10" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="28">
+        <v>0.97854785478547801</v>
+      </c>
+      <c r="D10" s="28">
+        <v>0.91612903225806397</v>
+      </c>
+      <c r="E10" s="28">
+        <v>0.85542168674698704</v>
+      </c>
+      <c r="F10" s="29">
+        <v>0.98611111111111105</v>
+      </c>
+      <c r="H10" s="23" t="str">
+        <f>VLOOKUP($B10,TL!$G10:$K27,1,FALSE)</f>
+        <v>KIRC</v>
+      </c>
+      <c r="I10" s="15">
+        <f>VLOOKUP($B10,TL!$G10:$K27,2,FALSE)</f>
+        <v>0.99504109650905481</v>
+      </c>
+      <c r="J10" s="15">
+        <f>VLOOKUP($B10,TL!$G10:$K27,3,FALSE)</f>
+        <v>0.97873357228195934</v>
+      </c>
+      <c r="K10" s="15">
+        <f>VLOOKUP($B10,TL!$G10:$K27,4,FALSE)</f>
+        <v>0.98750000000000004</v>
+      </c>
+      <c r="L10" s="15">
+        <f>VLOOKUP($B10,TL!$G10:$K27,5,FALSE)</f>
+        <v>0.97142857142857153</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B11" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="28">
+        <v>0.98142414860681104</v>
+      </c>
+      <c r="D11" s="28">
+        <v>0.91428571428571404</v>
+      </c>
+      <c r="E11" s="28">
+        <v>0.84210526315789402</v>
+      </c>
+      <c r="F11" s="29">
+        <v>1</v>
+      </c>
+      <c r="H11" s="23" t="e">
+        <f>VLOOKUP($B11,TL!$G11:$K28,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I11" s="15" t="e">
+        <f>VLOOKUP($B11,TL!$G11:$K28,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J11" s="15" t="e">
+        <f>VLOOKUP($B11,TL!$G11:$K28,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K11" s="15" t="e">
+        <f>VLOOKUP($B11,TL!$G11:$K28,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L11" s="15" t="e">
+        <f>VLOOKUP($B11,TL!$G11:$K28,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B12" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="28">
+        <v>0.93617021276595702</v>
+      </c>
+      <c r="D12" s="28">
+        <v>0.78740157480314898</v>
+      </c>
+      <c r="E12" s="28">
+        <v>0.64935064935064901</v>
+      </c>
+      <c r="F12" s="29">
+        <v>1</v>
+      </c>
+      <c r="H12" s="23" t="str">
+        <f>VLOOKUP($B12,TL!$G12:$K29,1,FALSE)</f>
+        <v>LIHC</v>
+      </c>
+      <c r="I12" s="15">
+        <f>VLOOKUP($B12,TL!$G12:$K29,2,FALSE)</f>
+        <v>0.9857983193277311</v>
+      </c>
+      <c r="J12" s="15">
+        <f>VLOOKUP($B12,TL!$G12:$K29,3,FALSE)</f>
+        <v>0.94071542492595128</v>
+      </c>
+      <c r="K12" s="15">
+        <f>VLOOKUP($B12,TL!$G12:$K29,4,FALSE)</f>
+        <v>0.92626262626262634</v>
+      </c>
+      <c r="L12" s="15">
+        <f>VLOOKUP($B12,TL!$G12:$K29,5,FALSE)</f>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B13" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="28">
+        <v>0.96701388888888795</v>
+      </c>
+      <c r="D13" s="28">
+        <v>0.86131386861313797</v>
+      </c>
+      <c r="E13" s="28">
+        <v>0.75641025641025605</v>
+      </c>
+      <c r="F13" s="29">
+        <v>1</v>
+      </c>
+      <c r="H13" s="23" t="e">
+        <f>VLOOKUP($B13,TL!$G13:$K30,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I13" s="15" t="e">
+        <f>VLOOKUP($B13,TL!$G13:$K30,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J13" s="15" t="e">
+        <f>VLOOKUP($B13,TL!$G13:$K30,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K13" s="15" t="e">
+        <f>VLOOKUP($B13,TL!$G13:$K30,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L13" s="15" t="e">
+        <f>VLOOKUP($B13,TL!$G13:$K30,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B14" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="28">
+        <v>0.98191681735985503</v>
+      </c>
+      <c r="D14" s="28">
+        <v>0.91071428571428503</v>
+      </c>
+      <c r="E14" s="28">
+        <v>0.83606557377049096</v>
+      </c>
+      <c r="F14" s="29">
+        <v>1</v>
+      </c>
+      <c r="H14" s="23" t="e">
+        <f>VLOOKUP($B14,TL!$G14:$K31,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I14" s="15" t="e">
+        <f>VLOOKUP($B14,TL!$G14:$K31,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J14" s="15" t="e">
+        <f>VLOOKUP($B14,TL!$G14:$K31,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K14" s="15" t="e">
+        <f>VLOOKUP($B14,TL!$G14:$K31,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L14" s="15" t="e">
+        <f>VLOOKUP($B14,TL!$G14:$K31,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B15" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="28">
+        <v>0.88545454545454505</v>
+      </c>
+      <c r="D15" s="28">
+        <v>0.56551724137931003</v>
+      </c>
+      <c r="E15" s="28">
+        <v>0.44086021505376299</v>
+      </c>
+      <c r="F15" s="29">
+        <v>0.78846153846153799</v>
+      </c>
+      <c r="H15" s="23" t="e">
+        <f>VLOOKUP($B15,TL!$G15:$K32,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I15" s="15" t="e">
+        <f>VLOOKUP($B15,TL!$G15:$K32,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J15" s="15" t="e">
+        <f>VLOOKUP($B15,TL!$G15:$K32,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K15" s="15" t="e">
+        <f>VLOOKUP($B15,TL!$G15:$K32,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L15" s="15" t="e">
+        <f>VLOOKUP($B15,TL!$G15:$K32,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B16" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="28">
+        <v>0.95777777777777695</v>
+      </c>
+      <c r="D16" s="28">
+        <v>0.78160919540229801</v>
+      </c>
+      <c r="E16" s="28">
+        <v>0.65384615384615297</v>
+      </c>
+      <c r="F16" s="29">
+        <v>0.97142857142857097</v>
+      </c>
+      <c r="H16" s="23" t="e">
+        <f>VLOOKUP($B16,TL!$G16:$K33,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I16" s="15" t="e">
+        <f>VLOOKUP($B16,TL!$G16:$K33,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J16" s="15" t="e">
+        <f>VLOOKUP($B16,TL!$G16:$K33,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K16" s="15" t="e">
+        <f>VLOOKUP($B16,TL!$G16:$K33,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L16" s="15" t="e">
+        <f>VLOOKUP($B16,TL!$G16:$K33,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="30">
+        <v>0.88461538461538403</v>
+      </c>
+      <c r="D17" s="30">
+        <v>0.63333333333333297</v>
+      </c>
+      <c r="E17" s="30">
+        <v>0.47107438016528902</v>
+      </c>
+      <c r="F17" s="18">
+        <v>0.96610169491525399</v>
+      </c>
+      <c r="H17" s="24" t="e">
+        <f>VLOOKUP($B17,TL!$G17:$K34,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I17" s="15" t="e">
+        <f>VLOOKUP($B17,TL!$G17:$K34,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J17" s="15" t="e">
+        <f>VLOOKUP($B17,TL!$G17:$K34,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K17" s="15" t="e">
+        <f>VLOOKUP($B17,TL!$G17:$K34,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L17" s="15" t="e">
+        <f>VLOOKUP($B17,TL!$G17:$K34,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" s="33" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+    </row>
+    <row r="25" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="B25" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B23:L23"/>
+    <mergeCell ref="B25:L25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
merged table is updated
</commit_message>
<xml_diff>
--- a/summary/performances.xlsx
+++ b/summary/performances.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10610"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucan\OneDrive - Politecnico di Milano\PhD\progetti\CIBB2018\summary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/canakoglu/GMQL-sources/CIBB2018/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64249C63-D71F-43A7-898D-F7691A32765F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{372FA923-4C9B-0845-9494-0A7132611FC8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16236" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCGA_info" sheetId="3" r:id="rId1"/>
@@ -27,12 +27,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Classical ML'!$A$2:$F$164</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TCGA_info!$A$2:$F$35</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="94">
   <si>
     <t>accuracy</t>
   </si>
@@ -235,30 +235,12 @@
     <t>%normal</t>
   </si>
   <si>
-    <t>DM</t>
-  </si>
-  <si>
-    <t>TRAN.LEARN</t>
-  </si>
-  <si>
-    <t>Ladder</t>
-  </si>
-  <si>
-    <t>AE</t>
-  </si>
-  <si>
-    <t>feature reduction</t>
-  </si>
-  <si>
     <t>LUAD + LUSC</t>
   </si>
   <si>
     <t>KIRC + KIRP + KICH</t>
   </si>
   <si>
-    <t>Data augmentation</t>
-  </si>
-  <si>
     <t>Additional information</t>
   </si>
   <si>
@@ -308,6 +290,35 @@
   </si>
   <si>
     <t>1vsALL</t>
+  </si>
+  <si>
+    <t>Data 
+augmentation</t>
+  </si>
+  <si>
+    <t>Feature
+reduction</t>
+  </si>
+  <si>
+    <t>Transfer
+Learning</t>
+  </si>
+  <si>
+    <t>Ladder
+Network</t>
+  </si>
+  <si>
+    <t>Distance
+ Matrix</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>In the supervised part of the algorithm there is only 60 samples used</t>
+  </si>
+  <si>
+    <t>5-CV</t>
   </si>
 </sst>
 </file>
@@ -409,7 +420,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -684,63 +695,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -759,9 +713,7 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top style="thick">
         <color auto="1"/>
       </top>
@@ -770,12 +722,105 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -824,7 +869,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -846,65 +906,61 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
-    <cellStyle name="Percentuale" xfId="1" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -922,7 +978,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1003,7 +1059,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1688,7 +1744,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="460990440"/>
@@ -1747,7 +1803,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="460991752"/>
@@ -1789,7 +1845,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1819,7 +1875,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2428,7 +2484,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2754,19 +2810,19 @@
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -2786,7 +2842,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
@@ -2807,7 +2863,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -2828,7 +2884,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -2849,7 +2905,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -2870,7 +2926,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -2891,7 +2947,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -2912,7 +2968,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -2933,7 +2989,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2954,7 +3010,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -2975,7 +3031,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -2996,7 +3052,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -3017,7 +3073,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -3038,7 +3094,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -3059,7 +3115,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -3080,7 +3136,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -3101,7 +3157,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -3122,7 +3178,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
@@ -3143,7 +3199,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -3164,7 +3220,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
@@ -3185,7 +3241,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
@@ -3206,7 +3262,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -3227,7 +3283,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -3248,7 +3304,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -3269,7 +3325,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -3290,7 +3346,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -3311,7 +3367,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>41</v>
       </c>
@@ -3332,7 +3388,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
@@ -3353,7 +3409,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
@@ -3374,7 +3430,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>17</v>
       </c>
@@ -3395,7 +3451,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -3416,7 +3472,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>18</v>
       </c>
@@ -3437,7 +3493,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -3458,7 +3514,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
@@ -3497,24 +3553,24 @@
       <selection activeCell="C2" sqref="C2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33.6" x14ac:dyDescent="0.65">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:6" ht="34" x14ac:dyDescent="0.4">
+      <c r="A1" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>54</v>
       </c>
@@ -3531,7 +3587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -3552,7 +3608,7 @@
         <v>0.93342783709138</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -3573,7 +3629,7 @@
         <v>0.98142897589386802</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -3594,7 +3650,7 @@
         <v>0.99254105839416051</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -3615,7 +3671,7 @@
         <v>0.99254105839416051</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -3636,7 +3692,7 @@
         <v>0.98743566479432654</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -3657,7 +3713,7 @@
         <v>0.99254105839416051</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3678,7 +3734,7 @@
         <v>0.9381888723275893</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -3699,7 +3755,7 @@
         <v>0.97280700799135544</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>16</v>
       </c>
@@ -3720,7 +3776,7 @@
         <v>0.9381888723275893</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>14</v>
       </c>
@@ -3741,7 +3797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -3762,7 +3818,7 @@
         <v>0.97963138493944213</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -3783,7 +3839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -3804,7 +3860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -3825,7 +3881,7 @@
         <v>0.98945470728207363</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -3846,7 +3902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -3867,7 +3923,7 @@
         <v>0.92121459900134073</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -3888,7 +3944,7 @@
         <v>0.93168869309838476</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>14</v>
       </c>
@@ -3909,7 +3965,7 @@
         <v>0.52585673349700923</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>15</v>
       </c>
@@ -3930,7 +3986,7 @@
         <v>0.97499191563499832</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
@@ -3951,7 +4007,7 @@
         <v>0.98916909853794277</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
@@ -3972,7 +4028,7 @@
         <v>0.99486998898126011</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
@@ -3993,7 +4049,7 @@
         <v>0.98538636911158961</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>15</v>
       </c>
@@ -4014,7 +4070,7 @@
         <v>0.99002149103971482</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>15</v>
       </c>
@@ -4035,7 +4091,7 @@
         <v>0.99316437262751078</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
@@ -4056,7 +4112,7 @@
         <v>0.81605696514016346</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
@@ -4077,7 +4133,7 @@
         <v>0.98871852244004577</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
         <v>15</v>
       </c>
@@ -4098,7 +4154,7 @@
         <v>0.77626543414849702</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
         <v>4</v>
       </c>
@@ -4119,7 +4175,7 @@
         <v>0.92431635321792094</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
@@ -4140,7 +4196,7 @@
         <v>0.98897028735473957</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
@@ -4161,7 +4217,7 @@
         <v>0.98834313662151152</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -4182,7 +4238,7 @@
         <v>0.96705553340674377</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>4</v>
       </c>
@@ -4203,7 +4259,7 @@
         <v>0.96832273162612936</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
@@ -4224,7 +4280,7 @@
         <v>0.98633392132871511</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>4</v>
       </c>
@@ -4245,7 +4301,7 @@
         <v>0.85548863352160343</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
@@ -4266,7 +4322,7 @@
         <v>0.98703726630069166</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
         <v>4</v>
       </c>
@@ -4287,7 +4343,7 @@
         <v>0.85016561387674594</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="23" t="s">
         <v>20</v>
       </c>
@@ -4308,7 +4364,7 @@
         <v>0.96198609045048045</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>20</v>
       </c>
@@ -4329,7 +4385,7 @@
         <v>0.99382000824292438</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>20</v>
       </c>
@@ -4350,7 +4406,7 @@
         <v>0.99197121344212535</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>20</v>
       </c>
@@ -4371,7 +4427,7 @@
         <v>0.98576496472925412</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>20</v>
       </c>
@@ -4392,7 +4448,7 @@
         <v>0.99153522929547155</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>20</v>
       </c>
@@ -4413,7 +4469,7 @@
         <v>0.99058216435555657</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>20</v>
       </c>
@@ -4434,7 +4490,7 @@
         <v>0.87536517239403921</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>20</v>
       </c>
@@ -4455,7 +4511,7 @@
         <v>0.99321064153036553</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
         <v>20</v>
       </c>
@@ -4476,7 +4532,7 @@
         <v>0.82063037762013002</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="23" t="s">
         <v>17</v>
       </c>
@@ -4497,7 +4553,7 @@
         <v>0.92171002978625005</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>17</v>
       </c>
@@ -4518,7 +4574,7 @@
         <v>0.96766016902440921</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>17</v>
       </c>
@@ -4539,7 +4595,7 @@
         <v>0.98715748983331675</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>17</v>
       </c>
@@ -4560,7 +4616,7 @@
         <v>0.97137312983436241</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>17</v>
       </c>
@@ -4581,7 +4637,7 @@
         <v>0.96564818113584405</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>17</v>
       </c>
@@ -4602,7 +4658,7 @@
         <v>0.98615413351303938</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>17</v>
       </c>
@@ -4623,7 +4679,7 @@
         <v>0.81614304813724192</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>17</v>
       </c>
@@ -4644,7 +4700,7 @@
         <v>0.99062747502826054</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
         <v>17</v>
       </c>
@@ -4665,7 +4721,7 @@
         <v>0.8017889383227903</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="23" t="s">
         <v>8</v>
       </c>
@@ -4686,7 +4742,7 @@
         <v>0.91491242479773871</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>8</v>
       </c>
@@ -4707,7 +4763,7 @@
         <v>0.98614668783411374</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>8</v>
       </c>
@@ -4728,7 +4784,7 @@
         <v>0.98846460022921379</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>8</v>
       </c>
@@ -4749,7 +4805,7 @@
         <v>0.97801665665891335</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>8</v>
       </c>
@@ -4770,7 +4826,7 @@
         <v>0.97938272361722756</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>8</v>
       </c>
@@ -4791,7 +4847,7 @@
         <v>0.98468794106606472</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>8</v>
       </c>
@@ -4812,7 +4868,7 @@
         <v>0.85048694279360326</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>8</v>
       </c>
@@ -4833,7 +4889,7 @@
         <v>0.99131757407630161</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="24" t="s">
         <v>8</v>
       </c>
@@ -4854,7 +4910,7 @@
         <v>0.85048694279360326</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="23" t="s">
         <v>5</v>
       </c>
@@ -4875,7 +4931,7 @@
         <v>0.96239078659640898</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>5</v>
       </c>
@@ -4896,7 +4952,7 @@
         <v>0.99475732424626429</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>5</v>
       </c>
@@ -4917,7 +4973,7 @@
         <v>0.99835895351950787</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>5</v>
       </c>
@@ -4938,7 +4994,7 @@
         <v>0.99275511386664239</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>5</v>
       </c>
@@ -4959,7 +5015,7 @@
         <v>0.99108386122525394</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>5</v>
       </c>
@@ -4980,7 +5036,7 @@
         <v>0.99475732424626429</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>5</v>
       </c>
@@ -5001,7 +5057,7 @@
         <v>0.82361801283346525</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>5</v>
       </c>
@@ -5022,7 +5078,7 @@
         <v>0.99475732424626429</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="24" t="s">
         <v>5</v>
       </c>
@@ -5043,7 +5099,7 @@
         <v>0.82414337994265474</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="23" t="s">
         <v>7</v>
       </c>
@@ -5064,7 +5120,7 @@
         <v>0.89229655899751925</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>7</v>
       </c>
@@ -5085,7 +5141,7 @@
         <v>0.9660568874430101</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>7</v>
       </c>
@@ -5106,7 +5162,7 @@
         <v>0.9577696454973843</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>7</v>
       </c>
@@ -5127,7 +5183,7 @@
         <v>0.9660568874430101</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>7</v>
       </c>
@@ -5148,7 +5204,7 @@
         <v>0.9567341492904996</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>7</v>
       </c>
@@ -5169,7 +5225,7 @@
         <v>0.9660568874430101</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>7</v>
       </c>
@@ -5190,7 +5246,7 @@
         <v>0.89042048439629262</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>7</v>
       </c>
@@ -5211,7 +5267,7 @@
         <v>0.9660568874430101</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="24" t="s">
         <v>7</v>
       </c>
@@ -5232,7 +5288,7 @@
         <v>0.89042048439629262</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="23" t="s">
         <v>12</v>
       </c>
@@ -5253,7 +5309,7 @@
         <v>0.91640477464424985</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>12</v>
       </c>
@@ -5274,7 +5330,7 @@
         <v>0.98183550520608875</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>12</v>
       </c>
@@ -5295,7 +5351,7 @@
         <v>0.98528676458249154</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>12</v>
       </c>
@@ -5316,7 +5372,7 @@
         <v>0.9634590798090622</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>12</v>
       </c>
@@ -5337,7 +5393,7 @@
         <v>0.98108671467625141</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>12</v>
       </c>
@@ -5358,7 +5414,7 @@
         <v>0.9762370260908031</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>12</v>
       </c>
@@ -5379,7 +5435,7 @@
         <v>0.91282094856419826</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>12</v>
       </c>
@@ -5400,7 +5456,7 @@
         <v>0.98727180486467481</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" s="24" t="s">
         <v>12</v>
       </c>
@@ -5421,7 +5477,7 @@
         <v>0.91282094856419826</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="23" t="s">
         <v>9</v>
       </c>
@@ -5442,7 +5498,7 @@
         <v>0.96122209165687411</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>9</v>
       </c>
@@ -5463,7 +5519,7 @@
         <v>0.97961697543188164</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>9</v>
       </c>
@@ -5484,7 +5540,7 @@
         <v>0.97643466086144881</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>9</v>
       </c>
@@ -5505,7 +5561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>9</v>
       </c>
@@ -5526,7 +5582,7 @@
         <v>0.97961697543188164</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>9</v>
       </c>
@@ -5547,7 +5603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>9</v>
       </c>
@@ -5568,7 +5624,7 @@
         <v>0.64080832382946129</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>9</v>
       </c>
@@ -5589,7 +5645,7 @@
         <v>0.97643466086144881</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="24" t="s">
         <v>9</v>
       </c>
@@ -5610,7 +5666,7 @@
         <v>0.64080832382946129</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="23" t="s">
         <v>6</v>
       </c>
@@ -5631,7 +5687,7 @@
         <v>0.89778791725507401</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>6</v>
       </c>
@@ -5652,7 +5708,7 @@
         <v>0.96752432456959747</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>6</v>
       </c>
@@ -5673,7 +5729,7 @@
         <v>0.94464249007298773</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>6</v>
       </c>
@@ -5694,7 +5750,7 @@
         <v>0.97637205875436972</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>6</v>
       </c>
@@ -5715,7 +5771,7 @@
         <v>0.90851454110602192</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>6</v>
       </c>
@@ -5736,7 +5792,7 @@
         <v>0.97637205875436972</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>6</v>
       </c>
@@ -5757,7 +5813,7 @@
         <v>0.8169378698224854</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>6</v>
       </c>
@@ -5778,7 +5834,7 @@
         <v>0.95070615658850921</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A110" s="24" t="s">
         <v>6</v>
       </c>
@@ -5799,7 +5855,7 @@
         <v>0.8169378698224854</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="23" t="s">
         <v>19</v>
       </c>
@@ -5820,7 +5876,7 @@
         <v>0.93743665785724206</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>19</v>
       </c>
@@ -5841,7 +5897,7 @@
         <v>0.97286426789261193</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>19</v>
       </c>
@@ -5862,7 +5918,7 @@
         <v>0.98679580934736344</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>19</v>
       </c>
@@ -5883,7 +5939,7 @@
         <v>0.97691381615327322</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>19</v>
       </c>
@@ -5904,7 +5960,7 @@
         <v>0.97192684674819696</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>19</v>
       </c>
@@ -5925,7 +5981,7 @@
         <v>0.98603599623958682</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>19</v>
       </c>
@@ -5946,7 +6002,7 @@
         <v>0.77629128560739868</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>19</v>
       </c>
@@ -5967,7 +6023,7 @@
         <v>0.98936080295385254</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A119" s="24" t="s">
         <v>19</v>
       </c>
@@ -5988,7 +6044,7 @@
         <v>0.7765653324345565</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="23" t="s">
         <v>10</v>
       </c>
@@ -6009,7 +6065,7 @@
         <v>0.96005973711686565</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>10</v>
       </c>
@@ -6030,7 +6086,7 @@
         <v>0.98890572330559889</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>10</v>
       </c>
@@ -6051,7 +6107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>10</v>
       </c>
@@ -6072,7 +6128,7 @@
         <v>0.98678761331293874</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>10</v>
       </c>
@@ -6093,7 +6149,7 @@
         <v>0.9873571748624258</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>10</v>
       </c>
@@ -6114,7 +6170,7 @@
         <v>0.9965384094072971</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>10</v>
       </c>
@@ -6135,7 +6191,7 @@
         <v>0.85060393827230385</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>10</v>
       </c>
@@ -6156,7 +6212,7 @@
         <v>0.98786282347320298</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A128" s="24" t="s">
         <v>10</v>
       </c>
@@ -6177,7 +6233,7 @@
         <v>0.81136396694210688</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" s="23" t="s">
         <v>11</v>
       </c>
@@ -6198,7 +6254,7 @@
         <v>0.94421131295178096</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>11</v>
       </c>
@@ -6219,7 +6275,7 @@
         <v>0.98882446624292764</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>11</v>
       </c>
@@ -6240,7 +6296,7 @@
         <v>0.99489049248364869</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>11</v>
       </c>
@@ -6261,7 +6317,7 @@
         <v>0.98432310695684699</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>11</v>
       </c>
@@ -6282,7 +6338,7 @@
         <v>0.97714184851486474</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>11</v>
       </c>
@@ -6303,7 +6359,7 @@
         <v>0.99302603186081362</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>11</v>
       </c>
@@ -6324,7 +6380,7 @@
         <v>0.80488224478401083</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>11</v>
       </c>
@@ -6345,7 +6401,7 @@
         <v>0.99105926706221448</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A137" s="24" t="s">
         <v>11</v>
       </c>
@@ -6366,7 +6422,7 @@
         <v>0.80505420565915642</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="23" t="s">
         <v>18</v>
       </c>
@@ -6387,7 +6443,7 @@
         <v>0.9548921682757836</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>18</v>
       </c>
@@ -6408,7 +6464,7 @@
         <v>0.9806545067282787</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>18</v>
       </c>
@@ -6429,7 +6485,7 @@
         <v>0.99460171405111342</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>18</v>
       </c>
@@ -6450,7 +6506,7 @@
         <v>0.95084223252771638</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>18</v>
       </c>
@@ -6471,7 +6527,7 @@
         <v>0.95670303502576992</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>18</v>
       </c>
@@ -6492,7 +6548,7 @@
         <v>0.97043400049102846</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>18</v>
       </c>
@@ -6513,7 +6569,7 @@
         <v>0.81789138020937768</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>18</v>
       </c>
@@ -6534,7 +6590,7 @@
         <v>0.95616610771904142</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A146" s="24" t="s">
         <v>18</v>
       </c>
@@ -6555,7 +6611,7 @@
         <v>0.77439999999999998</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="23" t="s">
         <v>13</v>
       </c>
@@ -6576,7 +6632,7 @@
         <v>0.91476528625700393</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>13</v>
       </c>
@@ -6597,7 +6653,7 @@
         <v>0.93961544570870492</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>13</v>
       </c>
@@ -6618,7 +6674,7 @@
         <v>0.95834112119603532</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>13</v>
       </c>
@@ -6639,7 +6695,7 @@
         <v>0.94753384827890708</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>13</v>
       </c>
@@ -6660,7 +6716,7 @@
         <v>0.932388471632563</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>13</v>
       </c>
@@ -6681,7 +6737,7 @@
         <v>0.93680233404510715</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>13</v>
       </c>
@@ -6702,7 +6758,7 @@
         <v>0.84748376126939884</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>13</v>
       </c>
@@ -6723,7 +6779,7 @@
         <v>0.9522372210146135</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A155" s="24" t="s">
         <v>13</v>
       </c>
@@ -6744,7 +6800,7 @@
         <v>0.81965971713983221</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="23" t="s">
         <v>21</v>
       </c>
@@ -6765,7 +6821,7 @@
         <v>0.96351497910408401</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>21</v>
       </c>
@@ -6786,7 +6842,7 @@
         <v>0.99711382965979867</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>21</v>
       </c>
@@ -6807,7 +6863,7 @@
         <v>0.9932262032858914</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>21</v>
       </c>
@@ -6828,7 +6884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>21</v>
       </c>
@@ -6849,7 +6905,7 @@
         <v>0.99314376869489918</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>21</v>
       </c>
@@ -6870,7 +6926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>21</v>
       </c>
@@ -6891,7 +6947,7 @@
         <v>0.78105198526807462</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>21</v>
       </c>
@@ -6912,7 +6968,7 @@
         <v>0.98472982708327028</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A164" s="24" t="s">
         <v>21</v>
       </c>
@@ -6951,42 +7007,42 @@
       <selection activeCell="B22" sqref="B22:E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="19" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="19" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:23" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="G1" s="37" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="G1" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="M1" s="37" t="s">
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="M1" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -7023,15 +7079,15 @@
       <c r="Q2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="39" t="s">
+      <c r="S2" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="39"/>
-      <c r="W2" s="39"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
+      <c r="V2" s="44"/>
+      <c r="W2" s="44"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -7078,7 +7134,7 @@
         <v>0.8727243452125375</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -7125,7 +7181,7 @@
         <v>0.94075163398692807</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -7172,35 +7228,35 @@
         <v>0.92877816627816634</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A6" s="43" t="s">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="44">
+      <c r="B6" s="34">
         <v>0.98474358974358966</v>
       </c>
-      <c r="C6" s="44">
+      <c r="C6" s="34">
         <v>0.89142857142857146</v>
       </c>
-      <c r="D6" s="44">
+      <c r="D6" s="34">
         <v>0.81666666666666665</v>
       </c>
-      <c r="E6" s="44">
-        <v>1</v>
-      </c>
-      <c r="G6" s="43" t="s">
+      <c r="E6" s="34">
+        <v>1</v>
+      </c>
+      <c r="G6" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="44">
+      <c r="H6" s="34">
         <v>0.98974358974358978</v>
       </c>
-      <c r="I6" s="44">
+      <c r="I6" s="34">
         <v>0.86666666666666659</v>
       </c>
-      <c r="J6" s="44">
-        <v>1</v>
-      </c>
-      <c r="K6" s="44">
+      <c r="J6" s="34">
+        <v>1</v>
+      </c>
+      <c r="K6" s="34">
         <v>0.8</v>
       </c>
       <c r="M6" s="1" t="s">
@@ -7219,7 +7275,7 @@
         <v>0.93029331779331792</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -7266,7 +7322,7 @@
         <v>0.92328224377020118</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -7313,7 +7369,7 @@
         <v>0.90674048174048172</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -7360,7 +7416,7 @@
         <v>0.92949640287769797</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -7407,35 +7463,35 @@
         <v>0.92057008192122092</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A11" s="43" t="s">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="44">
+      <c r="B11" s="34">
         <v>0.99299589603283178</v>
       </c>
-      <c r="C11" s="44">
+      <c r="C11" s="34">
         <v>0.93142857142857127</v>
       </c>
-      <c r="D11" s="44">
+      <c r="D11" s="34">
         <v>0.93333333333333324</v>
       </c>
-      <c r="E11" s="44">
+      <c r="E11" s="34">
         <v>0.95</v>
       </c>
-      <c r="G11" s="43" t="s">
+      <c r="G11" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="44">
+      <c r="H11" s="34">
         <v>0.98823464269428707</v>
       </c>
-      <c r="I11" s="44">
+      <c r="I11" s="34">
         <v>0.8571428571428571</v>
       </c>
-      <c r="J11" s="44">
+      <c r="J11" s="34">
         <v>0.88333333333333319</v>
       </c>
-      <c r="K11" s="44">
+      <c r="K11" s="34">
         <v>0.85</v>
       </c>
       <c r="M11" s="1" t="s">
@@ -7454,7 +7510,7 @@
         <v>0.95059434621915884</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -7501,7 +7557,7 @@
         <v>0.93925925925925924</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -7548,7 +7604,7 @@
         <v>0.93595744680851067</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -7595,7 +7651,7 @@
         <v>0.93129770992366423</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -7642,7 +7698,7 @@
         <v>0.96538314176245199</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -7689,7 +7745,7 @@
         <v>0.9207496352822353</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -7736,7 +7792,7 @@
         <v>0.87643363728470125</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -7783,35 +7839,35 @@
         <v>0.92742919389978229</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="43" t="s">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A19" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="44">
+      <c r="B19" s="34">
         <v>0.9909632841078444</v>
       </c>
-      <c r="C19" s="44">
+      <c r="C19" s="34">
         <v>0.95382269503546091</v>
       </c>
-      <c r="D19" s="44">
+      <c r="D19" s="34">
         <v>0.92031239935587761</v>
       </c>
-      <c r="E19" s="44">
+      <c r="E19" s="34">
         <v>0.99090909090909096</v>
       </c>
-      <c r="G19" s="43" t="s">
+      <c r="G19" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="44">
+      <c r="H19" s="34">
         <v>0.98851104186424599</v>
       </c>
-      <c r="I19" s="44">
+      <c r="I19" s="34">
         <v>0.94562199235649746</v>
       </c>
-      <c r="J19" s="44">
+      <c r="J19" s="34">
         <v>0.91041666666666676</v>
       </c>
-      <c r="K19" s="44">
+      <c r="K19" s="34">
         <v>0.9913043478260869</v>
       </c>
       <c r="M19" s="1" t="s">
@@ -7830,7 +7886,7 @@
         <v>0.93150739704118346</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -7877,9 +7933,9 @@
         <v>0.93585105257590173</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="42" t="s">
-        <v>72</v>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A21" s="32" t="s">
+        <v>67</v>
       </c>
       <c r="B21">
         <v>0.99397400000000002</v>
@@ -7893,8 +7949,8 @@
       <c r="E21">
         <v>0.99272700000000003</v>
       </c>
-      <c r="G21" s="42" t="s">
-        <v>72</v>
+      <c r="G21" s="32" t="s">
+        <v>67</v>
       </c>
       <c r="H21">
         <v>0.99503900000000001</v>
@@ -7909,9 +7965,9 @@
         <v>0.99636400000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B22">
         <v>0.99568299999999998</v>
@@ -7926,7 +7982,7 @@
         <v>0.98443099999999994</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H22">
         <v>0.99607900000000005</v>
@@ -7940,15 +7996,15 @@
       <c r="K22">
         <v>0.97981499999999999</v>
       </c>
-      <c r="M22" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="N22" s="41"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="41"/>
-      <c r="Q22" s="41"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="M22" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="N22" s="46"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="46"/>
+      <c r="Q22" s="46"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>4</v>
       </c>
@@ -8004,7 +8060,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -8063,7 +8119,7 @@
         <v>-3.0769230769230882E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>1</v>
       </c>
@@ -8122,7 +8178,7 @@
         <v>-1.1764705882352899E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>2</v>
       </c>
@@ -8181,7 +8237,7 @@
         <v>-2.222222222222214E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
@@ -8262,25 +8318,25 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="11" max="11" width="14.77734375" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="33.6" x14ac:dyDescent="0.65">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.4">
+      <c r="A1" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -8294,7 +8350,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -8310,15 +8366,15 @@
       <c r="E3">
         <v>0.97312299999999996</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
@@ -8335,7 +8391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>49</v>
       </c>
@@ -8352,25 +8408,25 @@
         <v>0.97692299999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="33.6" x14ac:dyDescent="0.65">
-      <c r="A9" s="35" t="s">
+    <row r="9" spans="1:10" ht="34" x14ac:dyDescent="0.4">
+      <c r="A9" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
         <v>0</v>
@@ -8392,7 +8448,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -8409,7 +8465,7 @@
         <v>0.98260899999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -8426,7 +8482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>49</v>
       </c>
@@ -8443,31 +8499,31 @@
         <v>0.99230799999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
     </row>
   </sheetData>
@@ -8489,26 +8545,26 @@
       <selection activeCell="C3" sqref="C3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:13" s="3" customFormat="1" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="37" t="s">
+    <row r="1" spans="2:13" s="3" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
       <c r="G1" s="22"/>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-    </row>
-    <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+    </row>
+    <row r="2" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="10"/>
       <c r="C2" s="20" t="s">
         <v>0</v>
@@ -8537,7 +8593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B3" s="11" t="s">
         <v>20</v>
       </c>
@@ -8574,7 +8630,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" s="12" t="s">
         <v>52</v>
       </c>
@@ -8611,7 +8667,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" s="12" t="s">
         <v>53</v>
       </c>
@@ -8648,14 +8704,14 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C15" s="20"/>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
@@ -8673,365 +8729,399 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0D92E8-BE8B-7042-85EF-6FE2473B88F2}">
-  <dimension ref="A1:R21"/>
+  <dimension ref="B1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B1" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="1" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:12" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="55"/>
+    </row>
+    <row r="3" spans="2:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="B3" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="G3" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="H3" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="J3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="O2" s="3" t="s">
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B4" s="58"/>
+      <c r="C4" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="18">
+        <v>0.9909632841078444</v>
+      </c>
+      <c r="E4" s="18">
+        <v>0.95382269503546091</v>
+      </c>
+      <c r="F4" s="18">
+        <v>0.92031239935587761</v>
+      </c>
+      <c r="G4" s="18">
+        <v>0.99090909090909096</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <v>0.99343599999999999</v>
+      </c>
+      <c r="J4">
+        <v>0.96574899999999997</v>
+      </c>
+      <c r="K4">
+        <v>0.95060900000000004</v>
+      </c>
+      <c r="L4">
+        <v>0.98260899999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B5" s="58"/>
+      <c r="C5" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="18">
+        <v>0.99397400000000002</v>
+      </c>
+      <c r="E5" s="18">
+        <v>0.97008700000000003</v>
+      </c>
+      <c r="F5" s="18">
+        <v>0.94891300000000001</v>
+      </c>
+      <c r="G5" s="18">
+        <v>0.99272700000000003</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5">
+        <v>0.99292000000000002</v>
+      </c>
+      <c r="J5">
+        <v>0.96574899999999997</v>
+      </c>
+      <c r="K5">
+        <v>0.93517300000000003</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="58"/>
+      <c r="C6" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6">
+        <v>0.99568299999999998</v>
+      </c>
+      <c r="E6">
+        <v>0.98293200000000003</v>
+      </c>
+      <c r="F6">
+        <v>0.98222699999999996</v>
+      </c>
+      <c r="G6">
+        <v>0.98443099999999994</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6">
+        <v>0.99803900000000001</v>
+      </c>
+      <c r="J6">
+        <v>0.99230499999999999</v>
+      </c>
+      <c r="K6">
+        <v>0.99259299999999995</v>
+      </c>
+      <c r="L6">
+        <v>0.99230799999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="31" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="45"/>
-      <c r="B3" s="1" t="s">
+      <c r="I7" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B8" s="60"/>
+      <c r="C8" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="18">
-        <v>0.9909632841078444</v>
-      </c>
-      <c r="D3" s="18">
-        <v>0.95382269503546091</v>
-      </c>
-      <c r="E3" s="18">
-        <v>0.92031239935587761</v>
-      </c>
-      <c r="F3" s="52">
-        <v>0.99090909090909096</v>
-      </c>
-      <c r="G3" s="47" t="s">
+      <c r="D8" s="18">
+        <v>0.99343599999999999</v>
+      </c>
+      <c r="E8" s="18">
+        <v>0.96574899999999997</v>
+      </c>
+      <c r="F8" s="18">
+        <v>0.95060900000000004</v>
+      </c>
+      <c r="G8" s="18">
+        <v>0.98260899999999995</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H3">
-        <v>0.99343599999999999</v>
-      </c>
-      <c r="I3">
-        <v>0.96574899999999997</v>
-      </c>
-      <c r="J3">
-        <v>0.95060900000000004</v>
-      </c>
-      <c r="K3">
-        <v>0.98260899999999995</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="N3" t="s">
-        <v>80</v>
-      </c>
-      <c r="O3" t="s">
-        <v>81</v>
-      </c>
-      <c r="P3" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>89</v>
-      </c>
-      <c r="R3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="45"/>
-      <c r="B4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="18">
-        <v>0.99397400000000002</v>
-      </c>
-      <c r="D4" s="18">
-        <v>0.97008700000000003</v>
-      </c>
-      <c r="E4" s="18">
-        <v>0.94891300000000001</v>
-      </c>
-      <c r="F4" s="52">
-        <v>0.99272700000000003</v>
-      </c>
-      <c r="G4" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4">
-        <v>0.99292000000000002</v>
-      </c>
-      <c r="I4">
-        <v>0.96574899999999997</v>
-      </c>
-      <c r="J4">
-        <v>0.93517300000000003</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="N4" t="s">
-        <v>80</v>
-      </c>
-      <c r="O4" t="s">
-        <v>81</v>
-      </c>
-      <c r="P4" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>89</v>
-      </c>
-      <c r="R4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="45"/>
-      <c r="B5" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5">
-        <v>0.99568299999999998</v>
-      </c>
-      <c r="D5">
-        <v>0.98293200000000003</v>
-      </c>
-      <c r="E5">
-        <v>0.98222699999999996</v>
-      </c>
-      <c r="F5">
-        <v>0.98443099999999994</v>
-      </c>
-      <c r="G5" s="54" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5">
-        <v>0.99803900000000001</v>
-      </c>
-      <c r="I5">
-        <v>0.99230499999999999</v>
-      </c>
-      <c r="J5">
-        <v>0.99259299999999995</v>
-      </c>
-      <c r="K5">
-        <v>0.99230799999999997</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="55" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="57" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="58" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="56" t="s">
-        <v>70</v>
-      </c>
-      <c r="H6" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="57" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="59"/>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="18">
-        <v>0.99343599999999999</v>
-      </c>
-      <c r="D7" s="18">
-        <v>0.96574899999999997</v>
-      </c>
-      <c r="E7" s="18">
-        <v>0.95060900000000004</v>
-      </c>
-      <c r="F7" s="52">
-        <v>0.98260899999999995</v>
-      </c>
-      <c r="G7" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="59"/>
-      <c r="B8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="18">
-        <v>0.99292000000000002</v>
-      </c>
-      <c r="D8" s="18">
-        <v>0.96574899999999997</v>
-      </c>
-      <c r="E8" s="18">
-        <v>0.93517300000000003</v>
-      </c>
-      <c r="F8" s="52">
-        <v>1</v>
-      </c>
-      <c r="G8" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="18"/>
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
       <c r="K8" s="18"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="59"/>
-      <c r="B9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="18">
-        <v>0.99803900000000001</v>
+      <c r="L8" s="18"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B9" s="60"/>
+      <c r="C9" s="35" t="s">
+        <v>46</v>
       </c>
       <c r="D9" s="18">
-        <v>0.99230499999999999</v>
+        <v>0.99292000000000002</v>
       </c>
       <c r="E9" s="18">
-        <v>0.99259299999999995</v>
-      </c>
-      <c r="F9" s="52">
-        <v>0.99230799999999997</v>
-      </c>
-      <c r="G9" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="18"/>
+        <v>0.96574899999999997</v>
+      </c>
+      <c r="F9" s="18">
+        <v>0.93517300000000003</v>
+      </c>
+      <c r="G9" s="18">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
+      <c r="L9" s="18"/>
+    </row>
+    <row r="10" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="61"/>
+      <c r="C10" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="18">
+        <v>0.99803900000000001</v>
+      </c>
+      <c r="E10" s="18">
+        <v>0.99230499999999999</v>
+      </c>
+      <c r="F10" s="18">
+        <v>0.99259299999999995</v>
+      </c>
+      <c r="G10" s="18">
+        <v>0.99230799999999997</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
corrected LN in the summary table
</commit_message>
<xml_diff>
--- a/summary/performances.xlsx
+++ b/summary/performances.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10610"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/canakoglu/GMQL-sources/CIBB2018/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{45C7BF39-EBC4-4C47-B6B9-269E9B28B2C4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DF86C58F-BFFF-0B4C-B337-56AB2CF4D2BE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCGA_info" sheetId="3" r:id="rId1"/>
@@ -909,6 +909,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -962,15 +971,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2828,14 +2828,14 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -3576,14 +3576,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="34" x14ac:dyDescent="0.4">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
@@ -7035,27 +7035,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="G1" s="48" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="G1" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="M1" s="48" t="s">
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="M1" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
@@ -7094,13 +7094,13 @@
       <c r="Q2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="50" t="s">
+      <c r="S2" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50"/>
-      <c r="V2" s="50"/>
-      <c r="W2" s="50"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -8011,13 +8011,13 @@
       <c r="K22">
         <v>0.97981499999999999</v>
       </c>
-      <c r="M22" s="51" t="s">
+      <c r="M22" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="N22" s="52"/>
-      <c r="O22" s="52"/>
-      <c r="P22" s="52"/>
-      <c r="Q22" s="52"/>
+      <c r="N22" s="55"/>
+      <c r="O22" s="55"/>
+      <c r="P22" s="55"/>
+      <c r="Q22" s="55"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
@@ -8343,13 +8343,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.4">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
@@ -8381,13 +8381,13 @@
       <c r="E3">
         <v>0.97312299999999996</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -8433,13 +8433,13 @@
       <c r="A8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="34" x14ac:dyDescent="0.4">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
@@ -8563,21 +8563,21 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:13" s="3" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
       <c r="G1" s="22"/>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
     </row>
     <row r="2" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="10"/>
@@ -8720,11 +8720,11 @@
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C15" s="20"/>
@@ -8747,7 +8747,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="I4" sqref="I4:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8767,23 +8767,23 @@
   <sheetData>
     <row r="1" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:14" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="59" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="61"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="64"/>
     </row>
     <row r="3" spans="2:14" ht="30" x14ac:dyDescent="0.2">
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="57" t="s">
         <v>86</v>
       </c>
       <c r="C3" s="43" t="s">
@@ -8818,7 +8818,7 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B4" s="55"/>
+      <c r="B4" s="58"/>
       <c r="C4" s="35" t="s">
         <v>20</v>
       </c>
@@ -8838,20 +8838,20 @@
         <v>20</v>
       </c>
       <c r="I4">
-        <v>0.99343599999999999</v>
+        <v>0.989326765188834</v>
       </c>
       <c r="J4">
-        <v>0.96574899999999997</v>
+        <v>0.94420600858369097</v>
       </c>
       <c r="K4">
-        <v>0.95060900000000004</v>
+        <v>0.92436974789915904</v>
       </c>
       <c r="L4">
-        <v>0.98260899999999995</v>
+        <v>0.96491228070175405</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B5" s="55"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="35" t="s">
         <v>46</v>
       </c>
@@ -8870,21 +8870,21 @@
       <c r="H5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I5">
-        <v>0.99292000000000002</v>
-      </c>
-      <c r="J5">
-        <v>0.96574899999999997</v>
-      </c>
-      <c r="K5">
-        <v>0.93517300000000003</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
+      <c r="I5" s="18">
+        <v>0.99019607843137203</v>
+      </c>
+      <c r="J5" s="18">
+        <v>0.96212121212121204</v>
+      </c>
+      <c r="K5" s="18">
+        <v>0.94074074074073999</v>
+      </c>
+      <c r="L5" s="19">
+        <v>0.98449612403100695</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="55"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="36" t="s">
         <v>49</v>
       </c>
@@ -8903,21 +8903,21 @@
       <c r="H6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I6">
-        <v>0.99803900000000001</v>
-      </c>
-      <c r="J6">
-        <v>0.99230499999999999</v>
-      </c>
-      <c r="K6">
-        <v>0.99259299999999995</v>
-      </c>
-      <c r="L6">
-        <v>0.99230799999999997</v>
+      <c r="I6" s="18">
+        <v>0.98317094774136404</v>
+      </c>
+      <c r="J6" s="18">
+        <v>0.92050209205020905</v>
+      </c>
+      <c r="K6" s="18">
+        <v>0.85271317829457305</v>
+      </c>
+      <c r="L6" s="19">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="31" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="59" t="s">
         <v>87</v>
       </c>
       <c r="C7" s="38" t="s">
@@ -8952,7 +8952,7 @@
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="57"/>
+      <c r="B8" s="60"/>
       <c r="C8" s="35" t="s">
         <v>20</v>
       </c>
@@ -8977,7 +8977,7 @@
       <c r="L8" s="18"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B9" s="57"/>
+      <c r="B9" s="60"/>
       <c r="C9" s="35" t="s">
         <v>46</v>
       </c>
@@ -9002,7 +9002,7 @@
       <c r="L9" s="18"/>
     </row>
     <row r="10" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="58"/>
+      <c r="B10" s="61"/>
       <c r="C10" s="36" t="s">
         <v>49</v>
       </c>
@@ -9027,45 +9027,45 @@
       <c r="L10" s="18"/>
     </row>
     <row r="11" spans="2:14" ht="26" x14ac:dyDescent="0.2">
-      <c r="B11" s="62"/>
-      <c r="C11" s="63"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
-      <c r="H11" s="63"/>
+      <c r="H11" s="45"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
     </row>
     <row r="12" spans="2:14" ht="26" x14ac:dyDescent="0.2">
-      <c r="B12" s="62"/>
-      <c r="C12" s="63"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="45"/>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
-      <c r="H12" s="63"/>
+      <c r="H12" s="45"/>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
     </row>
     <row r="13" spans="2:14" ht="26" x14ac:dyDescent="0.3">
-      <c r="B13" s="62"/>
-      <c r="C13" s="63"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="45"/>
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
-      <c r="H13" s="48" t="s">
+      <c r="H13" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="49"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="52"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.2">
       <c r="I14" s="1" t="s">
@@ -9221,7 +9221,7 @@
         <v>0.95747506139428284</v>
       </c>
       <c r="K21">
-        <f>(J21*L21)/(2*L21-J21)</f>
+        <f t="shared" ref="K21:K29" si="0">(J21*L21)/(2*L21-J21)</f>
         <v>0.96198609045048045</v>
       </c>
       <c r="L21">
@@ -9244,7 +9244,7 @@
       <c r="E22" t="s">
         <v>83</v>
       </c>
-      <c r="F22" s="64" t="s">
+      <c r="F22" s="46" t="s">
         <v>92</v>
       </c>
       <c r="H22" t="s">
@@ -9257,7 +9257,7 @@
         <v>0.99362105810153722</v>
       </c>
       <c r="K22">
-        <f>(J22*L22)/(2*L22-J22)</f>
+        <f t="shared" si="0"/>
         <v>0.99382000824292438</v>
       </c>
       <c r="L22">
@@ -9293,7 +9293,7 @@
         <v>0.99186341192441962</v>
       </c>
       <c r="K23">
-        <f>(J23*L23)/(2*L23-J23)</f>
+        <f t="shared" si="0"/>
         <v>0.99197121344212535</v>
       </c>
       <c r="L23">
@@ -9311,7 +9311,7 @@
         <v>0.98585728517050464</v>
       </c>
       <c r="K24">
-        <f>(J24*L24)/(2*L24-J24)</f>
+        <f t="shared" si="0"/>
         <v>0.98576496472925412</v>
       </c>
       <c r="L24">
@@ -9330,7 +9330,7 @@
         <v>0.99165563461807837</v>
       </c>
       <c r="K25">
-        <f>(J25*L25)/(2*L25-J25)</f>
+        <f t="shared" si="0"/>
         <v>0.99153522929547155</v>
       </c>
       <c r="L25">
@@ -9348,7 +9348,7 @@
         <v>0.99074537493195092</v>
       </c>
       <c r="K26">
-        <f>(J26*L26)/(2*L26-J26)</f>
+        <f t="shared" si="0"/>
         <v>0.99058216435555657</v>
       </c>
       <c r="L26">
@@ -9366,7 +9366,7 @@
         <v>0.89864567168925424</v>
       </c>
       <c r="K27">
-        <f>(J27*L27)/(2*L27-J27)</f>
+        <f t="shared" si="0"/>
         <v>0.87536517239403921</v>
       </c>
       <c r="L27">
@@ -9384,7 +9384,7 @@
         <v>0.99328908596412335</v>
       </c>
       <c r="K28">
-        <f>(J28*L28)/(2*L28-J28)</f>
+        <f t="shared" si="0"/>
         <v>0.99321064153036553</v>
       </c>
       <c r="L28">
@@ -9402,7 +9402,7 @@
         <v>0.86115187067185472</v>
       </c>
       <c r="K29" s="25">
-        <f>(J29*L29)/(2*L29-J29)</f>
+        <f t="shared" si="0"/>
         <v>0.82063037762013002</v>
       </c>
       <c r="L29" s="25">

</xml_diff>

<commit_message>
corrected autoencoder result to summary
</commit_message>
<xml_diff>
--- a/summary/performances.xlsx
+++ b/summary/performances.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucan\OneDrive - Politecnico di Milano\PhD\progetti\CIBB2018\summary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/canakoglu/GMQL-sources/CIBB2018/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BE1814-BCC0-4133-842B-6546D98E0ACF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4A44A723-8294-8849-B208-479547BF2AEF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16236" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCGA_info" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Classical ML'!$A$2:$F$164</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TCGA_info!$A$2:$F$35</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -974,8 +974,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
-    <cellStyle name="Percentuale" xfId="1" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -993,7 +993,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1074,7 +1074,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1759,7 +1759,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="460990440"/>
@@ -1818,7 +1818,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="460991752"/>
@@ -1860,7 +1860,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1890,7 +1890,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1904,7 +1904,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1966,7 +1966,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2222,6 +2222,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.95648604269293902</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.92205491585473798</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92352941176470504</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2285,7 +2294,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="547957640"/>
@@ -2344,7 +2353,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="547956000"/>
@@ -2386,7 +2395,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2423,7 +2432,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2437,7 +2446,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2499,7 +2508,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2755,6 +2764,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.71038251366120198</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33333333333333298</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.57142857142857095</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2818,7 +2836,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="547957640"/>
@@ -2877,7 +2895,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="547956000"/>
@@ -2919,7 +2937,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2956,7 +2974,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2970,7 +2988,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3032,7 +3050,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3288,6 +3306,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.94202898550724601</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98113207547169801</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3351,7 +3378,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="547957640"/>
@@ -3410,7 +3437,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="547956000"/>
@@ -3452,7 +3479,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3489,7 +3516,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3503,7 +3530,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3565,7 +3592,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3821,6 +3848,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.570175438596491</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.403100775193798</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3884,7 +3920,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="547957640"/>
@@ -3943,7 +3979,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="547956000"/>
@@ -3985,7 +4021,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4022,7 +4058,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6817,8 +6853,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="769620" y="7559040"/>
-          <a:ext cx="9616440" cy="6416040"/>
+          <a:off x="769620" y="7798394"/>
+          <a:ext cx="10785597" cy="6635453"/>
           <a:chOff x="769620" y="7559040"/>
           <a:chExt cx="9616440" cy="6416040"/>
         </a:xfrm>
@@ -6933,7 +6969,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7259,9 +7295,9 @@
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="47" t="s">
         <v>45</v>
       </c>
@@ -7271,7 +7307,7 @@
       <c r="E1" s="48"/>
       <c r="F1" s="48"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -7291,7 +7327,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
@@ -7312,7 +7348,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -7333,7 +7369,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -7354,7 +7390,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -7375,7 +7411,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -7396,7 +7432,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -7417,7 +7453,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -7438,7 +7474,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -7459,7 +7495,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -7480,7 +7516,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -7501,7 +7537,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -7522,7 +7558,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -7543,7 +7579,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -7564,7 +7600,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -7585,7 +7621,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -7606,7 +7642,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -7627,7 +7663,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
@@ -7648,7 +7684,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -7669,7 +7705,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
@@ -7690,7 +7726,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
@@ -7711,7 +7747,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -7732,7 +7768,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -7753,7 +7789,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -7774,7 +7810,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -7795,7 +7831,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -7816,7 +7852,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>41</v>
       </c>
@@ -7837,7 +7873,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
@@ -7858,7 +7894,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
@@ -7879,7 +7915,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>17</v>
       </c>
@@ -7900,7 +7936,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -7921,7 +7957,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>18</v>
       </c>
@@ -7942,7 +7978,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -7963,7 +7999,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
@@ -8002,14 +8038,14 @@
       <selection activeCell="E140" sqref="E140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:6" ht="34" x14ac:dyDescent="0.4">
       <c r="A1" s="49" t="s">
         <v>64</v>
       </c>
@@ -8019,7 +8055,7 @@
       <c r="E1" s="50"/>
       <c r="F1" s="50"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>54</v>
       </c>
@@ -8036,7 +8072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -8057,7 +8093,7 @@
         <v>0.93342783709138</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -8078,7 +8114,7 @@
         <v>0.98142897589386802</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -8099,7 +8135,7 @@
         <v>0.99254105839416051</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -8120,7 +8156,7 @@
         <v>0.99254105839416051</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -8141,7 +8177,7 @@
         <v>0.98743566479432654</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -8162,7 +8198,7 @@
         <v>0.99254105839416051</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -8183,7 +8219,7 @@
         <v>0.9381888723275893</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -8204,7 +8240,7 @@
         <v>0.97280700799135544</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>16</v>
       </c>
@@ -8225,7 +8261,7 @@
         <v>0.9381888723275893</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>14</v>
       </c>
@@ -8246,7 +8282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -8267,7 +8303,7 @@
         <v>0.97963138493944213</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -8288,7 +8324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -8309,7 +8345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -8330,7 +8366,7 @@
         <v>0.98945470728207363</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -8351,7 +8387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -8372,7 +8408,7 @@
         <v>0.92121459900134073</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -8393,7 +8429,7 @@
         <v>0.93168869309838476</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>14</v>
       </c>
@@ -8414,7 +8450,7 @@
         <v>0.52585673349700923</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>15</v>
       </c>
@@ -8435,7 +8471,7 @@
         <v>0.97499191563499832</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
@@ -8456,7 +8492,7 @@
         <v>0.98916909853794277</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
@@ -8477,7 +8513,7 @@
         <v>0.99486998898126011</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
@@ -8498,7 +8534,7 @@
         <v>0.98538636911158961</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>15</v>
       </c>
@@ -8519,7 +8555,7 @@
         <v>0.99002149103971482</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>15</v>
       </c>
@@ -8540,7 +8576,7 @@
         <v>0.99316437262751078</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
@@ -8561,7 +8597,7 @@
         <v>0.81605696514016346</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
@@ -8582,7 +8618,7 @@
         <v>0.98871852244004577</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
         <v>15</v>
       </c>
@@ -8603,7 +8639,7 @@
         <v>0.77626543414849702</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
         <v>4</v>
       </c>
@@ -8624,7 +8660,7 @@
         <v>0.92431635321792094</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
@@ -8645,7 +8681,7 @@
         <v>0.98897028735473957</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
@@ -8666,7 +8702,7 @@
         <v>0.98834313662151152</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -8687,7 +8723,7 @@
         <v>0.96705553340674377</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>4</v>
       </c>
@@ -8708,7 +8744,7 @@
         <v>0.96832273162612936</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
@@ -8729,7 +8765,7 @@
         <v>0.98633392132871511</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>4</v>
       </c>
@@ -8750,7 +8786,7 @@
         <v>0.85548863352160343</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
@@ -8771,7 +8807,7 @@
         <v>0.98703726630069166</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
         <v>4</v>
       </c>
@@ -8792,7 +8828,7 @@
         <v>0.85016561387674594</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="23" t="s">
         <v>20</v>
       </c>
@@ -8813,7 +8849,7 @@
         <v>0.96198609045048045</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>20</v>
       </c>
@@ -8834,7 +8870,7 @@
         <v>0.99382000824292438</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>20</v>
       </c>
@@ -8855,7 +8891,7 @@
         <v>0.99197121344212535</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>20</v>
       </c>
@@ -8876,7 +8912,7 @@
         <v>0.98576496472925412</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>20</v>
       </c>
@@ -8897,7 +8933,7 @@
         <v>0.99153522929547155</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>20</v>
       </c>
@@ -8918,7 +8954,7 @@
         <v>0.99058216435555657</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>20</v>
       </c>
@@ -8939,7 +8975,7 @@
         <v>0.87536517239403921</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>20</v>
       </c>
@@ -8960,7 +8996,7 @@
         <v>0.99321064153036553</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
         <v>20</v>
       </c>
@@ -8981,7 +9017,7 @@
         <v>0.82063037762013002</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="23" t="s">
         <v>17</v>
       </c>
@@ -9002,7 +9038,7 @@
         <v>0.92171002978625005</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>17</v>
       </c>
@@ -9023,7 +9059,7 @@
         <v>0.96766016902440921</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>17</v>
       </c>
@@ -9044,7 +9080,7 @@
         <v>0.98715748983331675</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>17</v>
       </c>
@@ -9065,7 +9101,7 @@
         <v>0.97137312983436241</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>17</v>
       </c>
@@ -9086,7 +9122,7 @@
         <v>0.96564818113584405</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>17</v>
       </c>
@@ -9107,7 +9143,7 @@
         <v>0.98615413351303938</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>17</v>
       </c>
@@ -9128,7 +9164,7 @@
         <v>0.81614304813724192</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>17</v>
       </c>
@@ -9149,7 +9185,7 @@
         <v>0.99062747502826054</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
         <v>17</v>
       </c>
@@ -9170,7 +9206,7 @@
         <v>0.8017889383227903</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="23" t="s">
         <v>8</v>
       </c>
@@ -9191,7 +9227,7 @@
         <v>0.91491242479773871</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>8</v>
       </c>
@@ -9212,7 +9248,7 @@
         <v>0.98614668783411374</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>8</v>
       </c>
@@ -9233,7 +9269,7 @@
         <v>0.98846460022921379</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>8</v>
       </c>
@@ -9254,7 +9290,7 @@
         <v>0.97801665665891335</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>8</v>
       </c>
@@ -9275,7 +9311,7 @@
         <v>0.97938272361722756</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>8</v>
       </c>
@@ -9296,7 +9332,7 @@
         <v>0.98468794106606472</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>8</v>
       </c>
@@ -9317,7 +9353,7 @@
         <v>0.85048694279360326</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>8</v>
       </c>
@@ -9338,7 +9374,7 @@
         <v>0.99131757407630161</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="24" t="s">
         <v>8</v>
       </c>
@@ -9359,7 +9395,7 @@
         <v>0.85048694279360326</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="23" t="s">
         <v>5</v>
       </c>
@@ -9380,7 +9416,7 @@
         <v>0.96239078659640898</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>5</v>
       </c>
@@ -9401,7 +9437,7 @@
         <v>0.99475732424626429</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>5</v>
       </c>
@@ -9422,7 +9458,7 @@
         <v>0.99835895351950787</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>5</v>
       </c>
@@ -9443,7 +9479,7 @@
         <v>0.99275511386664239</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>5</v>
       </c>
@@ -9464,7 +9500,7 @@
         <v>0.99108386122525394</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>5</v>
       </c>
@@ -9485,7 +9521,7 @@
         <v>0.99475732424626429</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>5</v>
       </c>
@@ -9506,7 +9542,7 @@
         <v>0.82361801283346525</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>5</v>
       </c>
@@ -9527,7 +9563,7 @@
         <v>0.99475732424626429</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="24" t="s">
         <v>5</v>
       </c>
@@ -9548,7 +9584,7 @@
         <v>0.82414337994265474</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="23" t="s">
         <v>7</v>
       </c>
@@ -9569,7 +9605,7 @@
         <v>0.89229655899751925</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>7</v>
       </c>
@@ -9590,7 +9626,7 @@
         <v>0.9660568874430101</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>7</v>
       </c>
@@ -9611,7 +9647,7 @@
         <v>0.9577696454973843</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>7</v>
       </c>
@@ -9632,7 +9668,7 @@
         <v>0.9660568874430101</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>7</v>
       </c>
@@ -9653,7 +9689,7 @@
         <v>0.9567341492904996</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>7</v>
       </c>
@@ -9674,7 +9710,7 @@
         <v>0.9660568874430101</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>7</v>
       </c>
@@ -9695,7 +9731,7 @@
         <v>0.89042048439629262</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>7</v>
       </c>
@@ -9716,7 +9752,7 @@
         <v>0.9660568874430101</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="24" t="s">
         <v>7</v>
       </c>
@@ -9737,7 +9773,7 @@
         <v>0.89042048439629262</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="23" t="s">
         <v>12</v>
       </c>
@@ -9758,7 +9794,7 @@
         <v>0.91640477464424985</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>12</v>
       </c>
@@ -9779,7 +9815,7 @@
         <v>0.98183550520608875</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>12</v>
       </c>
@@ -9800,7 +9836,7 @@
         <v>0.98528676458249154</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>12</v>
       </c>
@@ -9821,7 +9857,7 @@
         <v>0.9634590798090622</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>12</v>
       </c>
@@ -9842,7 +9878,7 @@
         <v>0.98108671467625141</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>12</v>
       </c>
@@ -9863,7 +9899,7 @@
         <v>0.9762370260908031</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>12</v>
       </c>
@@ -9884,7 +9920,7 @@
         <v>0.91282094856419826</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>12</v>
       </c>
@@ -9905,7 +9941,7 @@
         <v>0.98727180486467481</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" s="24" t="s">
         <v>12</v>
       </c>
@@ -9926,7 +9962,7 @@
         <v>0.91282094856419826</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="23" t="s">
         <v>9</v>
       </c>
@@ -9947,7 +9983,7 @@
         <v>0.96122209165687411</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>9</v>
       </c>
@@ -9968,7 +10004,7 @@
         <v>0.97961697543188164</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>9</v>
       </c>
@@ -9989,7 +10025,7 @@
         <v>0.97643466086144881</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>9</v>
       </c>
@@ -10010,7 +10046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>9</v>
       </c>
@@ -10031,7 +10067,7 @@
         <v>0.97961697543188164</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>9</v>
       </c>
@@ -10052,7 +10088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>9</v>
       </c>
@@ -10073,7 +10109,7 @@
         <v>0.64080832382946129</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>9</v>
       </c>
@@ -10094,7 +10130,7 @@
         <v>0.97643466086144881</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="24" t="s">
         <v>9</v>
       </c>
@@ -10115,7 +10151,7 @@
         <v>0.64080832382946129</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="23" t="s">
         <v>6</v>
       </c>
@@ -10136,7 +10172,7 @@
         <v>0.89778791725507401</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>6</v>
       </c>
@@ -10157,7 +10193,7 @@
         <v>0.96752432456959747</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>6</v>
       </c>
@@ -10178,7 +10214,7 @@
         <v>0.94464249007298773</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>6</v>
       </c>
@@ -10199,7 +10235,7 @@
         <v>0.97637205875436972</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>6</v>
       </c>
@@ -10220,7 +10256,7 @@
         <v>0.90851454110602192</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>6</v>
       </c>
@@ -10241,7 +10277,7 @@
         <v>0.97637205875436972</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>6</v>
       </c>
@@ -10262,7 +10298,7 @@
         <v>0.8169378698224854</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>6</v>
       </c>
@@ -10283,7 +10319,7 @@
         <v>0.95070615658850921</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A110" s="24" t="s">
         <v>6</v>
       </c>
@@ -10304,7 +10340,7 @@
         <v>0.8169378698224854</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="23" t="s">
         <v>19</v>
       </c>
@@ -10325,7 +10361,7 @@
         <v>0.93743665785724206</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>19</v>
       </c>
@@ -10346,7 +10382,7 @@
         <v>0.97286426789261193</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>19</v>
       </c>
@@ -10367,7 +10403,7 @@
         <v>0.98679580934736344</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>19</v>
       </c>
@@ -10388,7 +10424,7 @@
         <v>0.97691381615327322</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>19</v>
       </c>
@@ -10409,7 +10445,7 @@
         <v>0.97192684674819696</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>19</v>
       </c>
@@ -10430,7 +10466,7 @@
         <v>0.98603599623958682</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>19</v>
       </c>
@@ -10451,7 +10487,7 @@
         <v>0.77629128560739868</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>19</v>
       </c>
@@ -10472,7 +10508,7 @@
         <v>0.98936080295385254</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A119" s="24" t="s">
         <v>19</v>
       </c>
@@ -10493,7 +10529,7 @@
         <v>0.7765653324345565</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="23" t="s">
         <v>10</v>
       </c>
@@ -10514,7 +10550,7 @@
         <v>0.96005973711686565</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>10</v>
       </c>
@@ -10535,7 +10571,7 @@
         <v>0.98890572330559889</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>10</v>
       </c>
@@ -10556,7 +10592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>10</v>
       </c>
@@ -10577,7 +10613,7 @@
         <v>0.98678761331293874</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>10</v>
       </c>
@@ -10598,7 +10634,7 @@
         <v>0.9873571748624258</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>10</v>
       </c>
@@ -10619,7 +10655,7 @@
         <v>0.9965384094072971</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>10</v>
       </c>
@@ -10640,7 +10676,7 @@
         <v>0.85060393827230385</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>10</v>
       </c>
@@ -10661,7 +10697,7 @@
         <v>0.98786282347320298</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A128" s="24" t="s">
         <v>10</v>
       </c>
@@ -10682,7 +10718,7 @@
         <v>0.81136396694210688</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" s="23" t="s">
         <v>11</v>
       </c>
@@ -10703,7 +10739,7 @@
         <v>0.94421131295178096</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>11</v>
       </c>
@@ -10724,7 +10760,7 @@
         <v>0.98882446624292764</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>11</v>
       </c>
@@ -10745,7 +10781,7 @@
         <v>0.99489049248364869</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>11</v>
       </c>
@@ -10766,7 +10802,7 @@
         <v>0.98432310695684699</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>11</v>
       </c>
@@ -10787,7 +10823,7 @@
         <v>0.97714184851486474</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>11</v>
       </c>
@@ -10808,7 +10844,7 @@
         <v>0.99302603186081362</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>11</v>
       </c>
@@ -10829,7 +10865,7 @@
         <v>0.80488224478401083</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>11</v>
       </c>
@@ -10850,7 +10886,7 @@
         <v>0.99105926706221448</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A137" s="24" t="s">
         <v>11</v>
       </c>
@@ -10871,7 +10907,7 @@
         <v>0.80505420565915642</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="23" t="s">
         <v>18</v>
       </c>
@@ -10892,7 +10928,7 @@
         <v>0.9548921682757836</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>18</v>
       </c>
@@ -10913,7 +10949,7 @@
         <v>0.9806545067282787</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>18</v>
       </c>
@@ -10934,7 +10970,7 @@
         <v>0.99460171405111342</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>18</v>
       </c>
@@ -10955,7 +10991,7 @@
         <v>0.95084223252771638</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>18</v>
       </c>
@@ -10976,7 +11012,7 @@
         <v>0.95670303502576992</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>18</v>
       </c>
@@ -10997,7 +11033,7 @@
         <v>0.97043400049102846</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>18</v>
       </c>
@@ -11018,7 +11054,7 @@
         <v>0.81789138020937768</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>18</v>
       </c>
@@ -11039,7 +11075,7 @@
         <v>0.95616610771904142</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A146" s="24" t="s">
         <v>18</v>
       </c>
@@ -11060,7 +11096,7 @@
         <v>0.77439999999999998</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="23" t="s">
         <v>13</v>
       </c>
@@ -11081,7 +11117,7 @@
         <v>0.91476528625700393</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>13</v>
       </c>
@@ -11102,7 +11138,7 @@
         <v>0.93961544570870492</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>13</v>
       </c>
@@ -11123,7 +11159,7 @@
         <v>0.95834112119603532</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>13</v>
       </c>
@@ -11144,7 +11180,7 @@
         <v>0.94753384827890708</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>13</v>
       </c>
@@ -11165,7 +11201,7 @@
         <v>0.932388471632563</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>13</v>
       </c>
@@ -11186,7 +11222,7 @@
         <v>0.93680233404510715</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>13</v>
       </c>
@@ -11207,7 +11243,7 @@
         <v>0.84748376126939884</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>13</v>
       </c>
@@ -11228,7 +11264,7 @@
         <v>0.9522372210146135</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A155" s="24" t="s">
         <v>13</v>
       </c>
@@ -11249,7 +11285,7 @@
         <v>0.81965971713983221</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="23" t="s">
         <v>21</v>
       </c>
@@ -11270,7 +11306,7 @@
         <v>0.96351497910408401</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>21</v>
       </c>
@@ -11291,7 +11327,7 @@
         <v>0.99711382965979867</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>21</v>
       </c>
@@ -11312,7 +11348,7 @@
         <v>0.9932262032858914</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>21</v>
       </c>
@@ -11333,7 +11369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>21</v>
       </c>
@@ -11354,7 +11390,7 @@
         <v>0.99314376869489918</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>21</v>
       </c>
@@ -11375,7 +11411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>21</v>
       </c>
@@ -11396,7 +11432,7 @@
         <v>0.78105198526807462</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>21</v>
       </c>
@@ -11417,7 +11453,7 @@
         <v>0.98472982708327028</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A164" s="24" t="s">
         <v>21</v>
       </c>
@@ -11456,19 +11492,19 @@
       <selection activeCell="A6" activeCellId="2" sqref="A19:XFD19 A11:XFD11 A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="19" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="19" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:23" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="51" t="s">
         <v>22</v>
       </c>
@@ -11491,7 +11527,7 @@
       <c r="P1" s="52"/>
       <c r="Q1" s="52"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -11536,7 +11572,7 @@
       <c r="V2" s="53"/>
       <c r="W2" s="53"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -11583,7 +11619,7 @@
         <v>0.8727243452125375</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -11630,7 +11666,7 @@
         <v>0.94075163398692807</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -11677,7 +11713,7 @@
         <v>0.92877816627816634</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="33" t="s">
         <v>7</v>
       </c>
@@ -11724,7 +11760,7 @@
         <v>0.93029331779331792</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -11771,7 +11807,7 @@
         <v>0.92328224377020118</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -11818,7 +11854,7 @@
         <v>0.90674048174048172</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -11865,7 +11901,7 @@
         <v>0.92949640287769797</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -11912,7 +11948,7 @@
         <v>0.92057008192122092</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="33" t="s">
         <v>12</v>
       </c>
@@ -11959,7 +11995,7 @@
         <v>0.95059434621915884</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -12006,7 +12042,7 @@
         <v>0.93925925925925924</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -12053,7 +12089,7 @@
         <v>0.93595744680851067</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -12100,7 +12136,7 @@
         <v>0.93129770992366423</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -12147,7 +12183,7 @@
         <v>0.96538314176245199</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -12194,7 +12230,7 @@
         <v>0.9207496352822353</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -12241,7 +12277,7 @@
         <v>0.87643363728470125</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -12288,7 +12324,7 @@
         <v>0.92742919389978229</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="33" t="s">
         <v>20</v>
       </c>
@@ -12335,7 +12371,7 @@
         <v>0.93150739704118346</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -12382,7 +12418,7 @@
         <v>0.93585105257590173</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
         <v>67</v>
       </c>
@@ -12414,7 +12450,7 @@
         <v>0.99636400000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>68</v>
       </c>
@@ -12453,7 +12489,7 @@
       <c r="P22" s="55"/>
       <c r="Q22" s="55"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>4</v>
       </c>
@@ -12509,7 +12545,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -12568,7 +12604,7 @@
         <v>-3.0769230769230882E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>1</v>
       </c>
@@ -12627,7 +12663,7 @@
         <v>-1.1764705882352899E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>2</v>
       </c>
@@ -12686,7 +12722,7 @@
         <v>-2.222222222222214E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
@@ -12767,16 +12803,16 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="11" max="11" width="14.77734375" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.4">
       <c r="A1" s="49" t="s">
         <v>48</v>
       </c>
@@ -12785,7 +12821,7 @@
       <c r="D1" s="49"/>
       <c r="E1" s="49"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -12799,7 +12835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -12823,7 +12859,7 @@
       <c r="I3" s="53"/>
       <c r="J3" s="53"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
@@ -12840,7 +12876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>49</v>
       </c>
@@ -12857,16 +12893,16 @@
         <v>0.97692299999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:10" ht="34" x14ac:dyDescent="0.4">
       <c r="A9" s="49" t="s">
         <v>50</v>
       </c>
@@ -12875,7 +12911,7 @@
       <c r="D9" s="49"/>
       <c r="E9" s="49"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
         <v>0</v>
@@ -12897,7 +12933,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -12914,7 +12950,7 @@
         <v>0.98260899999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -12931,7 +12967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>49</v>
       </c>
@@ -12948,31 +12984,31 @@
         <v>0.99230799999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
     </row>
   </sheetData>
@@ -12994,9 +13030,9 @@
       <selection activeCell="C3" sqref="C3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:13" s="3" customFormat="1" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:13" s="3" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="51" t="s">
         <v>65</v>
       </c>
@@ -13013,7 +13049,7 @@
       <c r="L1" s="52"/>
       <c r="M1" s="52"/>
     </row>
-    <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="10"/>
       <c r="C2" s="20" t="s">
         <v>0</v>
@@ -13042,7 +13078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B3" s="11" t="s">
         <v>20</v>
       </c>
@@ -13079,7 +13115,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" s="12" t="s">
         <v>52</v>
       </c>
@@ -13116,7 +13152,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" s="12" t="s">
         <v>53</v>
       </c>
@@ -13153,14 +13189,14 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" s="56"/>
       <c r="C13" s="56"/>
       <c r="D13" s="56"/>
       <c r="E13" s="56"/>
       <c r="F13" s="56"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C15" s="20"/>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
@@ -13180,27 +13216,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0D92E8-BE8B-7042-85EF-6FE2473B88F2}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="N37" sqref="N37"/>
+    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="188" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
     <col min="9" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:14" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:14" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C2" s="62" t="s">
         <v>69</v>
       </c>
@@ -13216,7 +13252,7 @@
       <c r="K2" s="63"/>
       <c r="L2" s="64"/>
     </row>
-    <row r="3" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" ht="30" x14ac:dyDescent="0.2">
       <c r="B3" s="57" t="s">
         <v>86</v>
       </c>
@@ -13251,7 +13287,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B4" s="58"/>
       <c r="C4" s="35" t="s">
         <v>20</v>
@@ -13284,7 +13320,7 @@
         <v>0.96491228070175405</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B5" s="58"/>
       <c r="C5" s="35" t="s">
         <v>46</v>
@@ -13317,7 +13353,7 @@
         <v>0.98449612403100695</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="58"/>
       <c r="C6" s="36" t="s">
         <v>49</v>
@@ -13350,7 +13386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" ht="31" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B7" s="59" t="s">
         <v>87</v>
       </c>
@@ -13385,7 +13421,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B8" s="60"/>
       <c r="C8" s="35" t="s">
         <v>20</v>
@@ -13405,12 +13441,20 @@
       <c r="H8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="I8" s="18">
+        <v>0.95648604269293902</v>
+      </c>
+      <c r="J8" s="18">
+        <v>0.71038251366120198</v>
+      </c>
+      <c r="K8" s="18">
+        <v>0.94202898550724601</v>
+      </c>
+      <c r="L8" s="18">
+        <v>0.570175438596491</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B9" s="60"/>
       <c r="C9" s="35" t="s">
         <v>46</v>
@@ -13430,12 +13474,20 @@
       <c r="H9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-    </row>
-    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I9" s="18">
+        <v>0.92205491585473798</v>
+      </c>
+      <c r="J9" s="18">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="K9" s="18">
+        <v>1</v>
+      </c>
+      <c r="L9" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="61"/>
       <c r="C10" s="36" t="s">
         <v>49</v>
@@ -13455,12 +13507,20 @@
       <c r="H10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-    </row>
-    <row r="11" spans="2:14" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="I10" s="18">
+        <v>0.92352941176470504</v>
+      </c>
+      <c r="J10" s="18">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="K10" s="18">
+        <v>0.98113207547169801</v>
+      </c>
+      <c r="L10" s="18">
+        <v>0.403100775193798</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="26" x14ac:dyDescent="0.2">
       <c r="B11" s="44"/>
       <c r="C11" s="45"/>
       <c r="D11" s="18"/>
@@ -13473,7 +13533,7 @@
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
     </row>
-    <row r="12" spans="2:14" ht="25.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14" ht="26" x14ac:dyDescent="0.2">
       <c r="B12" s="44"/>
       <c r="C12" s="45"/>
       <c r="D12" s="18"/>
@@ -13486,7 +13546,7 @@
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
     </row>
-    <row r="13" spans="2:14" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:14" ht="26" x14ac:dyDescent="0.3">
       <c r="B13" s="44"/>
       <c r="C13" s="45"/>
       <c r="D13" s="18"/>
@@ -13501,7 +13561,7 @@
       <c r="K13" s="52"/>
       <c r="L13" s="52"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
       <c r="I14" s="1" t="s">
         <v>0</v>
       </c>
@@ -13518,7 +13578,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
       <c r="H15" s="1" t="s">
         <v>20</v>
       </c>
@@ -13535,7 +13595,7 @@
         <v>0.9913043478260869</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
       <c r="H16" s="1" t="s">
         <v>46</v>
       </c>
@@ -13552,7 +13612,7 @@
         <v>0.99636400000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H17" s="5" t="s">
         <v>49</v>
       </c>
@@ -13569,14 +13629,14 @@
         <v>0.97981499999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>72</v>
@@ -13594,7 +13654,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>71</v>
       </c>
@@ -13626,7 +13686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>77</v>
       </c>
@@ -13662,7 +13722,7 @@
         <v>0.95300614189585864</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>78</v>
       </c>
@@ -13701,7 +13761,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>79</v>
       </c>
@@ -13734,7 +13794,7 @@
         <v>0.9917556338346204</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H24" t="s">
         <v>58</v>
       </c>
@@ -13752,7 +13812,7 @@
         <v>0.9859496229056588</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B25" s="3"/>
       <c r="H25" t="s">
         <v>59</v>
@@ -13771,7 +13831,7 @@
         <v>0.9917760691866504</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H26" t="s">
         <v>60</v>
       </c>
@@ -13789,7 +13849,7 @@
         <v>0.99090863929910145</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H27" t="s">
         <v>61</v>
       </c>
@@ -13807,7 +13867,7 @@
         <v>0.92319830194643915</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H28" t="s">
         <v>62</v>
       </c>
@@ -13825,7 +13885,7 @@
         <v>0.99336754279004658</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H29" s="25" t="s">
         <v>63</v>
       </c>
@@ -13852,6 +13912,7 @@
     <mergeCell ref="H13:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added NN to plots
</commit_message>
<xml_diff>
--- a/summary/performances.xlsx
+++ b/summary/performances.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/canakoglu/GMQL-sources/CIBB2018/summary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucan\OneDrive - Politecnico di Milano\PhD\progetti\CIBB2018\summary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4A44A723-8294-8849-B208-479547BF2AEF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="6_{451907C7-AB60-4BB7-A014-F4FB3421056D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{6D86615D-EA27-4160-B803-0E94256B8DC2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16236" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCGA_info" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Classical ML'!$A$2:$F$164</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TCGA_info!$A$2:$F$35</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -974,8 +974,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Percentuale" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -993,7 +993,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1074,7 +1074,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1759,7 +1759,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="460990440"/>
@@ -1818,7 +1818,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="460991752"/>
@@ -1860,7 +1860,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1890,7 +1890,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="it-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1904,7 +1904,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1966,7 +1966,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2004,7 +2004,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$8:$H$10</c:f>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2070,7 +2070,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$8:$H$10</c:f>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2136,7 +2136,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$8:$H$10</c:f>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2201,7 +2201,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$8:$H$10</c:f>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2237,6 +2237,63 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000F-DF54-4DF6-AE17-39DCCDE510CB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>FFNN</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>BRCA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>LUAD+LUSC</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KIRC+KIRP+KICH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Merged table'!$I$15:$I$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.98851104186424599</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99503900000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99607900000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B134-41D3-9850-062EEC6D8A2D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2294,7 +2351,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="547957640"/>
@@ -2353,7 +2410,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="547956000"/>
@@ -2395,7 +2452,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2432,7 +2489,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="it-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2446,7 +2503,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2508,7 +2565,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2546,7 +2603,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$8:$H$10</c:f>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2612,7 +2669,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$8:$H$10</c:f>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2678,7 +2735,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$8:$H$10</c:f>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2743,7 +2800,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$8:$H$10</c:f>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2779,6 +2836,63 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-34CF-4D3A-A36C-8A38E3E8042D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>FFNN</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>BRCA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>LUAD+LUSC</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KIRC+KIRP+KICH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Merged table'!$J$15:$J$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.94562199235649746</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97575999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98426599999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-145A-46FF-8B95-AE8B6E1E8E5F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2836,7 +2950,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="547957640"/>
@@ -2895,7 +3009,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="547956000"/>
@@ -2937,7 +3051,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2974,7 +3088,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="it-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2988,7 +3102,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3050,7 +3164,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3088,7 +3202,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$8:$H$10</c:f>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3154,7 +3268,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$8:$H$10</c:f>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3220,7 +3334,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$8:$H$10</c:f>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3285,7 +3399,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$8:$H$10</c:f>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3321,6 +3435,63 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-42F9-4B2E-8B7B-909E1159D05D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>FFNN</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>BRCA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>LUAD+LUSC</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KIRC+KIRP+KICH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Merged table'!$K$15:$K$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.91041666666666676</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95708099999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98945899999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-92C3-45D3-9EE5-BB168E9F8112}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3378,7 +3549,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="547957640"/>
@@ -3437,7 +3608,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="547956000"/>
@@ -3479,7 +3650,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3516,7 +3687,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="it-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3530,7 +3701,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3592,7 +3763,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3630,7 +3801,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$8:$H$10</c:f>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3696,7 +3867,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$8:$H$10</c:f>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3762,7 +3933,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$8:$H$10</c:f>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3827,7 +3998,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$8:$H$10</c:f>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3863,6 +4034,63 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-6795-474A-AF60-A4490CBB64BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>FFNN</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>BRCA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>LUAD+LUSC</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KIRC+KIRP+KICH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Merged table'!$L$15:$L$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.9913043478260869</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99636400000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97981499999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CB45-4816-A4D6-21C0E44C220E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3920,7 +4148,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="547957640"/>
@@ -3979,7 +4207,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="547956000"/>
@@ -4021,7 +4249,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4058,7 +4286,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="it-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6832,7 +7060,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>769620</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>83819</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
@@ -6853,10 +7081,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="769620" y="7798394"/>
-          <a:ext cx="10785597" cy="6635453"/>
-          <a:chOff x="769620" y="7559040"/>
-          <a:chExt cx="9616440" cy="6416040"/>
+          <a:off x="769620" y="7617680"/>
+          <a:ext cx="9612133" cy="6508806"/>
+          <a:chOff x="769620" y="7559039"/>
+          <a:chExt cx="9616440" cy="6416041"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:graphicFrame macro="">
@@ -6894,7 +7122,7 @@
           </xdr:cNvGraphicFramePr>
         </xdr:nvGraphicFramePr>
         <xdr:xfrm>
-          <a:off x="5798820" y="7559040"/>
+          <a:off x="5798820" y="7559039"/>
           <a:ext cx="4572000" cy="3017520"/>
         </xdr:xfrm>
         <a:graphic>
@@ -6969,7 +7197,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7295,9 +7523,9 @@
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="47" t="s">
         <v>45</v>
       </c>
@@ -7307,7 +7535,7 @@
       <c r="E1" s="48"/>
       <c r="F1" s="48"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -7327,7 +7555,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
@@ -7348,7 +7576,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -7369,7 +7597,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -7390,7 +7618,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -7411,7 +7639,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -7432,7 +7660,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -7453,7 +7681,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -7474,7 +7702,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -7495,7 +7723,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -7516,7 +7744,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -7537,7 +7765,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -7558,7 +7786,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -7579,7 +7807,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -7600,7 +7828,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -7621,7 +7849,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -7642,7 +7870,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -7663,7 +7891,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
@@ -7684,7 +7912,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -7705,7 +7933,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
@@ -7726,7 +7954,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
@@ -7747,7 +7975,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -7768,7 +7996,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -7789,7 +8017,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -7810,7 +8038,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -7831,7 +8059,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -7852,7 +8080,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>41</v>
       </c>
@@ -7873,7 +8101,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
@@ -7894,7 +8122,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
@@ -7915,7 +8143,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>17</v>
       </c>
@@ -7936,7 +8164,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -7957,7 +8185,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>18</v>
       </c>
@@ -7978,7 +8206,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -7999,7 +8227,7 @@
         <v>20530</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
@@ -8038,14 +8266,14 @@
       <selection activeCell="E140" sqref="E140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="34" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="33.6" x14ac:dyDescent="0.65">
       <c r="A1" s="49" t="s">
         <v>64</v>
       </c>
@@ -8055,7 +8283,7 @@
       <c r="E1" s="50"/>
       <c r="F1" s="50"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>54</v>
       </c>
@@ -8072,7 +8300,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -8093,7 +8321,7 @@
         <v>0.93342783709138</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -8114,7 +8342,7 @@
         <v>0.98142897589386802</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -8135,7 +8363,7 @@
         <v>0.99254105839416051</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -8156,7 +8384,7 @@
         <v>0.99254105839416051</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -8177,7 +8405,7 @@
         <v>0.98743566479432654</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -8198,7 +8426,7 @@
         <v>0.99254105839416051</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -8219,7 +8447,7 @@
         <v>0.9381888723275893</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -8240,7 +8468,7 @@
         <v>0.97280700799135544</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="24" t="s">
         <v>16</v>
       </c>
@@ -8261,7 +8489,7 @@
         <v>0.9381888723275893</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
         <v>14</v>
       </c>
@@ -8282,7 +8510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -8303,7 +8531,7 @@
         <v>0.97963138493944213</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -8324,7 +8552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -8345,7 +8573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -8366,7 +8594,7 @@
         <v>0.98945470728207363</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -8387,7 +8615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -8408,7 +8636,7 @@
         <v>0.92121459900134073</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -8429,7 +8657,7 @@
         <v>0.93168869309838476</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="24" t="s">
         <v>14</v>
       </c>
@@ -8450,7 +8678,7 @@
         <v>0.52585673349700923</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="23" t="s">
         <v>15</v>
       </c>
@@ -8471,7 +8699,7 @@
         <v>0.97499191563499832</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
@@ -8492,7 +8720,7 @@
         <v>0.98916909853794277</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
@@ -8513,7 +8741,7 @@
         <v>0.99486998898126011</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
@@ -8534,7 +8762,7 @@
         <v>0.98538636911158961</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>15</v>
       </c>
@@ -8555,7 +8783,7 @@
         <v>0.99002149103971482</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>15</v>
       </c>
@@ -8576,7 +8804,7 @@
         <v>0.99316437262751078</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
@@ -8597,7 +8825,7 @@
         <v>0.81605696514016346</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
@@ -8618,7 +8846,7 @@
         <v>0.98871852244004577</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="24" t="s">
         <v>15</v>
       </c>
@@ -8639,7 +8867,7 @@
         <v>0.77626543414849702</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="23" t="s">
         <v>4</v>
       </c>
@@ -8660,7 +8888,7 @@
         <v>0.92431635321792094</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
@@ -8681,7 +8909,7 @@
         <v>0.98897028735473957</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
@@ -8702,7 +8930,7 @@
         <v>0.98834313662151152</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -8723,7 +8951,7 @@
         <v>0.96705553340674377</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>4</v>
       </c>
@@ -8744,7 +8972,7 @@
         <v>0.96832273162612936</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
@@ -8765,7 +8993,7 @@
         <v>0.98633392132871511</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>4</v>
       </c>
@@ -8786,7 +9014,7 @@
         <v>0.85548863352160343</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
@@ -8807,7 +9035,7 @@
         <v>0.98703726630069166</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="24" t="s">
         <v>4</v>
       </c>
@@ -8828,7 +9056,7 @@
         <v>0.85016561387674594</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="23" t="s">
         <v>20</v>
       </c>
@@ -8849,7 +9077,7 @@
         <v>0.96198609045048045</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>20</v>
       </c>
@@ -8870,7 +9098,7 @@
         <v>0.99382000824292438</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>20</v>
       </c>
@@ -8891,7 +9119,7 @@
         <v>0.99197121344212535</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>20</v>
       </c>
@@ -8912,7 +9140,7 @@
         <v>0.98576496472925412</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>20</v>
       </c>
@@ -8933,7 +9161,7 @@
         <v>0.99153522929547155</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>20</v>
       </c>
@@ -8954,7 +9182,7 @@
         <v>0.99058216435555657</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>20</v>
       </c>
@@ -8975,7 +9203,7 @@
         <v>0.87536517239403921</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>20</v>
       </c>
@@ -8996,7 +9224,7 @@
         <v>0.99321064153036553</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="24" t="s">
         <v>20</v>
       </c>
@@ -9017,7 +9245,7 @@
         <v>0.82063037762013002</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="23" t="s">
         <v>17</v>
       </c>
@@ -9038,7 +9266,7 @@
         <v>0.92171002978625005</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>17</v>
       </c>
@@ -9059,7 +9287,7 @@
         <v>0.96766016902440921</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>17</v>
       </c>
@@ -9080,7 +9308,7 @@
         <v>0.98715748983331675</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>17</v>
       </c>
@@ -9101,7 +9329,7 @@
         <v>0.97137312983436241</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>17</v>
       </c>
@@ -9122,7 +9350,7 @@
         <v>0.96564818113584405</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>17</v>
       </c>
@@ -9143,7 +9371,7 @@
         <v>0.98615413351303938</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>17</v>
       </c>
@@ -9164,7 +9392,7 @@
         <v>0.81614304813724192</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>17</v>
       </c>
@@ -9185,7 +9413,7 @@
         <v>0.99062747502826054</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="24" t="s">
         <v>17</v>
       </c>
@@ -9206,7 +9434,7 @@
         <v>0.8017889383227903</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="23" t="s">
         <v>8</v>
       </c>
@@ -9227,7 +9455,7 @@
         <v>0.91491242479773871</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>8</v>
       </c>
@@ -9248,7 +9476,7 @@
         <v>0.98614668783411374</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>8</v>
       </c>
@@ -9269,7 +9497,7 @@
         <v>0.98846460022921379</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>8</v>
       </c>
@@ -9290,7 +9518,7 @@
         <v>0.97801665665891335</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>8</v>
       </c>
@@ -9311,7 +9539,7 @@
         <v>0.97938272361722756</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>8</v>
       </c>
@@ -9332,7 +9560,7 @@
         <v>0.98468794106606472</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>8</v>
       </c>
@@ -9353,7 +9581,7 @@
         <v>0.85048694279360326</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>8</v>
       </c>
@@ -9374,7 +9602,7 @@
         <v>0.99131757407630161</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="24" t="s">
         <v>8</v>
       </c>
@@ -9395,7 +9623,7 @@
         <v>0.85048694279360326</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="23" t="s">
         <v>5</v>
       </c>
@@ -9416,7 +9644,7 @@
         <v>0.96239078659640898</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>5</v>
       </c>
@@ -9437,7 +9665,7 @@
         <v>0.99475732424626429</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>5</v>
       </c>
@@ -9458,7 +9686,7 @@
         <v>0.99835895351950787</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>5</v>
       </c>
@@ -9479,7 +9707,7 @@
         <v>0.99275511386664239</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>5</v>
       </c>
@@ -9500,7 +9728,7 @@
         <v>0.99108386122525394</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>5</v>
       </c>
@@ -9521,7 +9749,7 @@
         <v>0.99475732424626429</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>5</v>
       </c>
@@ -9542,7 +9770,7 @@
         <v>0.82361801283346525</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>5</v>
       </c>
@@ -9563,7 +9791,7 @@
         <v>0.99475732424626429</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="24" t="s">
         <v>5</v>
       </c>
@@ -9584,7 +9812,7 @@
         <v>0.82414337994265474</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="23" t="s">
         <v>7</v>
       </c>
@@ -9605,7 +9833,7 @@
         <v>0.89229655899751925</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>7</v>
       </c>
@@ -9626,7 +9854,7 @@
         <v>0.9660568874430101</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>7</v>
       </c>
@@ -9647,7 +9875,7 @@
         <v>0.9577696454973843</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>7</v>
       </c>
@@ -9668,7 +9896,7 @@
         <v>0.9660568874430101</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>7</v>
       </c>
@@ -9689,7 +9917,7 @@
         <v>0.9567341492904996</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>7</v>
       </c>
@@ -9710,7 +9938,7 @@
         <v>0.9660568874430101</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>7</v>
       </c>
@@ -9731,7 +9959,7 @@
         <v>0.89042048439629262</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>7</v>
       </c>
@@ -9752,7 +9980,7 @@
         <v>0.9660568874430101</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="24" t="s">
         <v>7</v>
       </c>
@@ -9773,7 +10001,7 @@
         <v>0.89042048439629262</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="23" t="s">
         <v>12</v>
       </c>
@@ -9794,7 +10022,7 @@
         <v>0.91640477464424985</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>12</v>
       </c>
@@ -9815,7 +10043,7 @@
         <v>0.98183550520608875</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>12</v>
       </c>
@@ -9836,7 +10064,7 @@
         <v>0.98528676458249154</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>12</v>
       </c>
@@ -9857,7 +10085,7 @@
         <v>0.9634590798090622</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>12</v>
       </c>
@@ -9878,7 +10106,7 @@
         <v>0.98108671467625141</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>12</v>
       </c>
@@ -9899,7 +10127,7 @@
         <v>0.9762370260908031</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>12</v>
       </c>
@@ -9920,7 +10148,7 @@
         <v>0.91282094856419826</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>12</v>
       </c>
@@ -9941,7 +10169,7 @@
         <v>0.98727180486467481</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="24" t="s">
         <v>12</v>
       </c>
@@ -9962,7 +10190,7 @@
         <v>0.91282094856419826</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="23" t="s">
         <v>9</v>
       </c>
@@ -9983,7 +10211,7 @@
         <v>0.96122209165687411</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>9</v>
       </c>
@@ -10004,7 +10232,7 @@
         <v>0.97961697543188164</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>9</v>
       </c>
@@ -10025,7 +10253,7 @@
         <v>0.97643466086144881</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>9</v>
       </c>
@@ -10046,7 +10274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>9</v>
       </c>
@@ -10067,7 +10295,7 @@
         <v>0.97961697543188164</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>9</v>
       </c>
@@ -10088,7 +10316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>9</v>
       </c>
@@ -10109,7 +10337,7 @@
         <v>0.64080832382946129</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>9</v>
       </c>
@@ -10130,7 +10358,7 @@
         <v>0.97643466086144881</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="24" t="s">
         <v>9</v>
       </c>
@@ -10151,7 +10379,7 @@
         <v>0.64080832382946129</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="23" t="s">
         <v>6</v>
       </c>
@@ -10172,7 +10400,7 @@
         <v>0.89778791725507401</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>6</v>
       </c>
@@ -10193,7 +10421,7 @@
         <v>0.96752432456959747</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>6</v>
       </c>
@@ -10214,7 +10442,7 @@
         <v>0.94464249007298773</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>6</v>
       </c>
@@ -10235,7 +10463,7 @@
         <v>0.97637205875436972</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>6</v>
       </c>
@@ -10256,7 +10484,7 @@
         <v>0.90851454110602192</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>6</v>
       </c>
@@ -10277,7 +10505,7 @@
         <v>0.97637205875436972</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>6</v>
       </c>
@@ -10298,7 +10526,7 @@
         <v>0.8169378698224854</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>6</v>
       </c>
@@ -10319,7 +10547,7 @@
         <v>0.95070615658850921</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="24" t="s">
         <v>6</v>
       </c>
@@ -10340,7 +10568,7 @@
         <v>0.8169378698224854</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="23" t="s">
         <v>19</v>
       </c>
@@ -10361,7 +10589,7 @@
         <v>0.93743665785724206</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>19</v>
       </c>
@@ -10382,7 +10610,7 @@
         <v>0.97286426789261193</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>19</v>
       </c>
@@ -10403,7 +10631,7 @@
         <v>0.98679580934736344</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>19</v>
       </c>
@@ -10424,7 +10652,7 @@
         <v>0.97691381615327322</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>19</v>
       </c>
@@ -10445,7 +10673,7 @@
         <v>0.97192684674819696</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>19</v>
       </c>
@@ -10466,7 +10694,7 @@
         <v>0.98603599623958682</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>19</v>
       </c>
@@ -10487,7 +10715,7 @@
         <v>0.77629128560739868</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>19</v>
       </c>
@@ -10508,7 +10736,7 @@
         <v>0.98936080295385254</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="24" t="s">
         <v>19</v>
       </c>
@@ -10529,7 +10757,7 @@
         <v>0.7765653324345565</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="23" t="s">
         <v>10</v>
       </c>
@@ -10550,7 +10778,7 @@
         <v>0.96005973711686565</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>10</v>
       </c>
@@ -10571,7 +10799,7 @@
         <v>0.98890572330559889</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>10</v>
       </c>
@@ -10592,7 +10820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>10</v>
       </c>
@@ -10613,7 +10841,7 @@
         <v>0.98678761331293874</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>10</v>
       </c>
@@ -10634,7 +10862,7 @@
         <v>0.9873571748624258</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>10</v>
       </c>
@@ -10655,7 +10883,7 @@
         <v>0.9965384094072971</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>10</v>
       </c>
@@ -10676,7 +10904,7 @@
         <v>0.85060393827230385</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>10</v>
       </c>
@@ -10697,7 +10925,7 @@
         <v>0.98786282347320298</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="24" t="s">
         <v>10</v>
       </c>
@@ -10718,7 +10946,7 @@
         <v>0.81136396694210688</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="23" t="s">
         <v>11</v>
       </c>
@@ -10739,7 +10967,7 @@
         <v>0.94421131295178096</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>11</v>
       </c>
@@ -10760,7 +10988,7 @@
         <v>0.98882446624292764</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>11</v>
       </c>
@@ -10781,7 +11009,7 @@
         <v>0.99489049248364869</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>11</v>
       </c>
@@ -10802,7 +11030,7 @@
         <v>0.98432310695684699</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>11</v>
       </c>
@@ -10823,7 +11051,7 @@
         <v>0.97714184851486474</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>11</v>
       </c>
@@ -10844,7 +11072,7 @@
         <v>0.99302603186081362</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>11</v>
       </c>
@@ -10865,7 +11093,7 @@
         <v>0.80488224478401083</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>11</v>
       </c>
@@ -10886,7 +11114,7 @@
         <v>0.99105926706221448</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A137" s="24" t="s">
         <v>11</v>
       </c>
@@ -10907,7 +11135,7 @@
         <v>0.80505420565915642</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="23" t="s">
         <v>18</v>
       </c>
@@ -10928,7 +11156,7 @@
         <v>0.9548921682757836</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>18</v>
       </c>
@@ -10949,7 +11177,7 @@
         <v>0.9806545067282787</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>18</v>
       </c>
@@ -10970,7 +11198,7 @@
         <v>0.99460171405111342</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>18</v>
       </c>
@@ -10991,7 +11219,7 @@
         <v>0.95084223252771638</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>18</v>
       </c>
@@ -11012,7 +11240,7 @@
         <v>0.95670303502576992</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>18</v>
       </c>
@@ -11033,7 +11261,7 @@
         <v>0.97043400049102846</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>18</v>
       </c>
@@ -11054,7 +11282,7 @@
         <v>0.81789138020937768</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>18</v>
       </c>
@@ -11075,7 +11303,7 @@
         <v>0.95616610771904142</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="24" t="s">
         <v>18</v>
       </c>
@@ -11096,7 +11324,7 @@
         <v>0.77439999999999998</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="23" t="s">
         <v>13</v>
       </c>
@@ -11117,7 +11345,7 @@
         <v>0.91476528625700393</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>13</v>
       </c>
@@ -11138,7 +11366,7 @@
         <v>0.93961544570870492</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>13</v>
       </c>
@@ -11159,7 +11387,7 @@
         <v>0.95834112119603532</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>13</v>
       </c>
@@ -11180,7 +11408,7 @@
         <v>0.94753384827890708</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>13</v>
       </c>
@@ -11201,7 +11429,7 @@
         <v>0.932388471632563</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>13</v>
       </c>
@@ -11222,7 +11450,7 @@
         <v>0.93680233404510715</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>13</v>
       </c>
@@ -11243,7 +11471,7 @@
         <v>0.84748376126939884</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>13</v>
       </c>
@@ -11264,7 +11492,7 @@
         <v>0.9522372210146135</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A155" s="24" t="s">
         <v>13</v>
       </c>
@@ -11285,7 +11513,7 @@
         <v>0.81965971713983221</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" s="23" t="s">
         <v>21</v>
       </c>
@@ -11306,7 +11534,7 @@
         <v>0.96351497910408401</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>21</v>
       </c>
@@ -11327,7 +11555,7 @@
         <v>0.99711382965979867</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>21</v>
       </c>
@@ -11348,7 +11576,7 @@
         <v>0.9932262032858914</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>21</v>
       </c>
@@ -11369,7 +11597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>21</v>
       </c>
@@ -11390,7 +11618,7 @@
         <v>0.99314376869489918</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>21</v>
       </c>
@@ -11411,7 +11639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>21</v>
       </c>
@@ -11432,7 +11660,7 @@
         <v>0.78105198526807462</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>21</v>
       </c>
@@ -11453,7 +11681,7 @@
         <v>0.98472982708327028</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A164" s="24" t="s">
         <v>21</v>
       </c>
@@ -11492,19 +11720,19 @@
       <selection activeCell="A6" activeCellId="2" sqref="A19:XFD19 A11:XFD11 A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="19" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="19" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="2" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="51" t="s">
         <v>22</v>
       </c>
@@ -11527,7 +11755,7 @@
       <c r="P1" s="52"/>
       <c r="Q1" s="52"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -11572,7 +11800,7 @@
       <c r="V2" s="53"/>
       <c r="W2" s="53"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -11619,7 +11847,7 @@
         <v>0.8727243452125375</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -11666,7 +11894,7 @@
         <v>0.94075163398692807</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -11713,7 +11941,7 @@
         <v>0.92877816627816634</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
         <v>7</v>
       </c>
@@ -11760,7 +11988,7 @@
         <v>0.93029331779331792</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -11807,7 +12035,7 @@
         <v>0.92328224377020118</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -11854,7 +12082,7 @@
         <v>0.90674048174048172</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -11901,7 +12129,7 @@
         <v>0.92949640287769797</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -11948,7 +12176,7 @@
         <v>0.92057008192122092</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="33" t="s">
         <v>12</v>
       </c>
@@ -11995,7 +12223,7 @@
         <v>0.95059434621915884</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -12042,7 +12270,7 @@
         <v>0.93925925925925924</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -12089,7 +12317,7 @@
         <v>0.93595744680851067</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -12136,7 +12364,7 @@
         <v>0.93129770992366423</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -12183,7 +12411,7 @@
         <v>0.96538314176245199</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -12230,7 +12458,7 @@
         <v>0.9207496352822353</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -12277,7 +12505,7 @@
         <v>0.87643363728470125</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -12324,7 +12552,7 @@
         <v>0.92742919389978229</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="33" t="s">
         <v>20</v>
       </c>
@@ -12371,7 +12599,7 @@
         <v>0.93150739704118346</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -12418,7 +12646,7 @@
         <v>0.93585105257590173</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="32" t="s">
         <v>67</v>
       </c>
@@ -12450,7 +12678,7 @@
         <v>0.99636400000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>68</v>
       </c>
@@ -12489,7 +12717,7 @@
       <c r="P22" s="55"/>
       <c r="Q22" s="55"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>4</v>
       </c>
@@ -12545,7 +12773,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -12604,7 +12832,7 @@
         <v>-3.0769230769230882E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>1</v>
       </c>
@@ -12663,7 +12891,7 @@
         <v>-1.1764705882352899E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>2</v>
       </c>
@@ -12722,7 +12950,7 @@
         <v>-2.222222222222214E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
@@ -12803,16 +13031,16 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="11" max="11" width="14.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="33.6" x14ac:dyDescent="0.65">
       <c r="A1" s="49" t="s">
         <v>48</v>
       </c>
@@ -12821,7 +13049,7 @@
       <c r="D1" s="49"/>
       <c r="E1" s="49"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -12835,7 +13063,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -12859,7 +13087,7 @@
       <c r="I3" s="53"/>
       <c r="J3" s="53"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
@@ -12876,7 +13104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>49</v>
       </c>
@@ -12893,16 +13121,16 @@
         <v>0.97692299999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="34" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="33.6" x14ac:dyDescent="0.65">
       <c r="A9" s="49" t="s">
         <v>50</v>
       </c>
@@ -12911,7 +13139,7 @@
       <c r="D9" s="49"/>
       <c r="E9" s="49"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
         <v>0</v>
@@ -12933,7 +13161,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -12950,7 +13178,7 @@
         <v>0.98260899999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -12967,7 +13195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>49</v>
       </c>
@@ -12984,31 +13212,31 @@
         <v>0.99230799999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
     </row>
   </sheetData>
@@ -13030,9 +13258,9 @@
       <selection activeCell="C3" sqref="C3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:13" s="3" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:13" s="3" customFormat="1" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="51" t="s">
         <v>65</v>
       </c>
@@ -13049,7 +13277,7 @@
       <c r="L1" s="52"/>
       <c r="M1" s="52"/>
     </row>
-    <row r="2" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="10"/>
       <c r="C2" s="20" t="s">
         <v>0</v>
@@ -13078,7 +13306,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
         <v>20</v>
       </c>
@@ -13115,7 +13343,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
         <v>52</v>
       </c>
@@ -13152,7 +13380,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="12" t="s">
         <v>53</v>
       </c>
@@ -13189,14 +13417,14 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" s="56"/>
       <c r="C13" s="56"/>
       <c r="D13" s="56"/>
       <c r="E13" s="56"/>
       <c r="F13" s="56"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C15" s="20"/>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
@@ -13216,27 +13444,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0D92E8-BE8B-7042-85EF-6FE2473B88F2}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="188" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
     <col min="9" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:14" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:14" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="62" t="s">
         <v>69</v>
       </c>
@@ -13252,7 +13480,7 @@
       <c r="K2" s="63"/>
       <c r="L2" s="64"/>
     </row>
-    <row r="3" spans="2:14" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="57" t="s">
         <v>86</v>
       </c>
@@ -13287,7 +13515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" s="58"/>
       <c r="C4" s="35" t="s">
         <v>20</v>
@@ -13320,7 +13548,7 @@
         <v>0.96491228070175405</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="58"/>
       <c r="C5" s="35" t="s">
         <v>46</v>
@@ -13353,7 +13581,7 @@
         <v>0.98449612403100695</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="58"/>
       <c r="C6" s="36" t="s">
         <v>49</v>
@@ -13386,7 +13614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="31" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:14" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B7" s="59" t="s">
         <v>87</v>
       </c>
@@ -13421,7 +13649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="60"/>
       <c r="C8" s="35" t="s">
         <v>20</v>
@@ -13454,7 +13682,7 @@
         <v>0.570175438596491</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="60"/>
       <c r="C9" s="35" t="s">
         <v>46</v>
@@ -13487,7 +13715,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="61"/>
       <c r="C10" s="36" t="s">
         <v>49</v>
@@ -13520,7 +13748,7 @@
         <v>0.403100775193798</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="26" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:14" ht="25.8" x14ac:dyDescent="0.3">
       <c r="B11" s="44"/>
       <c r="C11" s="45"/>
       <c r="D11" s="18"/>
@@ -13533,7 +13761,7 @@
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
     </row>
-    <row r="12" spans="2:14" ht="26" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:14" ht="25.8" x14ac:dyDescent="0.3">
       <c r="B12" s="44"/>
       <c r="C12" s="45"/>
       <c r="D12" s="18"/>
@@ -13546,7 +13774,7 @@
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
     </row>
-    <row r="13" spans="2:14" ht="26" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B13" s="44"/>
       <c r="C13" s="45"/>
       <c r="D13" s="18"/>
@@ -13561,7 +13789,7 @@
       <c r="K13" s="52"/>
       <c r="L13" s="52"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="I14" s="1" t="s">
         <v>0</v>
       </c>
@@ -13578,7 +13806,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="H15" s="1" t="s">
         <v>20</v>
       </c>
@@ -13595,7 +13823,7 @@
         <v>0.9913043478260869</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="H16" s="1" t="s">
         <v>46</v>
       </c>
@@ -13612,7 +13840,7 @@
         <v>0.99636400000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H17" s="5" t="s">
         <v>49</v>
       </c>
@@ -13629,14 +13857,14 @@
         <v>0.97981499999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>72</v>
@@ -13654,7 +13882,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>71</v>
       </c>
@@ -13686,7 +13914,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>77</v>
       </c>
@@ -13722,7 +13950,7 @@
         <v>0.95300614189585864</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>78</v>
       </c>
@@ -13761,7 +13989,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>79</v>
       </c>
@@ -13794,7 +14022,7 @@
         <v>0.9917556338346204</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H24" t="s">
         <v>58</v>
       </c>
@@ -13812,7 +14040,7 @@
         <v>0.9859496229056588</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B25" s="3"/>
       <c r="H25" t="s">
         <v>59</v>
@@ -13831,7 +14059,7 @@
         <v>0.9917760691866504</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H26" t="s">
         <v>60</v>
       </c>
@@ -13849,7 +14077,7 @@
         <v>0.99090863929910145</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H27" t="s">
         <v>61</v>
       </c>
@@ -13867,7 +14095,7 @@
         <v>0.92319830194643915</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H28" t="s">
         <v>62</v>
       </c>
@@ -13885,7 +14113,7 @@
         <v>0.99336754279004658</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H29" s="25" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
added LinearSVM to plots
</commit_message>
<xml_diff>
--- a/summary/performances.xlsx
+++ b/summary/performances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucan\OneDrive - Politecnico di Milano\PhD\progetti\CIBB2018\summary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="6_{451907C7-AB60-4BB7-A014-F4FB3421056D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{6D86615D-EA27-4160-B803-0E94256B8DC2}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="6_{451907C7-AB60-4BB7-A014-F4FB3421056D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{CCC14476-A39C-47FD-A318-50A911518322}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16236" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,12 +27,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Classical ML'!$A$2:$F$164</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TCGA_info!$A$2:$F$35</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="97">
   <si>
     <t>accuracy</t>
   </si>
@@ -321,10 +321,13 @@
     <t>5-CV</t>
   </si>
   <si>
-    <t xml:space="preserve"> calculate LUNG AND KIDNEY</t>
+    <t>FFNN</t>
   </si>
   <si>
-    <t>TL against NN</t>
+    <t>LinearSVM</t>
+  </si>
+  <si>
+    <t>Baselines</t>
   </si>
 </sst>
 </file>
@@ -426,7 +429,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -821,12 +824,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -970,6 +986,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2004,7 +2034,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2070,7 +2100,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2136,7 +2166,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2201,7 +2231,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2258,7 +2288,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2294,6 +2324,71 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B134-41D3-9850-062EEC6D8A2D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Merged table'!$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LinearSVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>BRCA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>LUAD+LUSC</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KIRC+KIRP+KICH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Merged table'!$D$15:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.99491300000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99698600000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.996668</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-07D8-4D93-9B99-FBA8EF467B3E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2603,7 +2698,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2669,7 +2764,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2735,7 +2830,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2800,7 +2895,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2857,7 +2952,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2893,6 +2988,71 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-145A-46FF-8B95-AE8B6E1E8E5F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Merged table'!$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LinearSVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>BRCA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>LUAD+LUSC</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KIRC+KIRP+KICH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Merged table'!$E$15:$E$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.97324100000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98484700000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98686499999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C01D-403E-98BA-3A658E936328}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3202,7 +3362,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3268,7 +3428,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3334,7 +3494,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3399,7 +3559,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3456,7 +3616,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3492,6 +3652,71 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-92C3-45D3-9EE5-BB168E9F8112}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Merged table'!$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LinearSVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>BRCA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>LUAD+LUSC</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KIRC+KIRP+KICH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Merged table'!$F$15:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.96469899999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97389999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98830300000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5439-4D94-B458-3CA3C67EABC8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3801,7 +4026,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3867,7 +4092,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3933,7 +4158,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3998,7 +4223,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -4055,7 +4280,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Merged table'!$H$15:$H$17</c:f>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -4091,6 +4316,71 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-CB45-4816-A4D6-21C0E44C220E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Merged table'!$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LinearSVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Merged table'!$C$15:$C$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>BRCA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>LUAD+LUSC</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KIRC+KIRP+KICH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Merged table'!$G$15:$G$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.98260899999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99636400000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98603099999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1872-49F7-8BC4-048222C28E1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7081,8 +7371,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="769620" y="7617680"/>
-          <a:ext cx="9612133" cy="6508806"/>
+          <a:off x="769620" y="7611054"/>
+          <a:ext cx="10188603" cy="6508806"/>
           <a:chOff x="769620" y="7559039"/>
           <a:chExt cx="9616440" cy="6416041"/>
         </a:xfrm>
@@ -13442,17 +13732,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0D92E8-BE8B-7042-85EF-6FE2473B88F2}">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K74" sqref="K74"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.44140625" customWidth="1"/>
@@ -13463,8 +13754,8 @@
     <col min="19" max="19" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:14" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:12" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="62" t="s">
         <v>69</v>
       </c>
@@ -13480,7 +13771,7 @@
       <c r="K2" s="63"/>
       <c r="L2" s="64"/>
     </row>
-    <row r="3" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="57" t="s">
         <v>86</v>
       </c>
@@ -13515,7 +13806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="58"/>
       <c r="C4" s="35" t="s">
         <v>20</v>
@@ -13548,7 +13839,7 @@
         <v>0.96491228070175405</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="58"/>
       <c r="C5" s="35" t="s">
         <v>46</v>
@@ -13581,7 +13872,7 @@
         <v>0.98449612403100695</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="58"/>
       <c r="C6" s="36" t="s">
         <v>49</v>
@@ -13614,7 +13905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B7" s="59" t="s">
         <v>87</v>
       </c>
@@ -13649,7 +13940,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="60"/>
       <c r="C8" s="35" t="s">
         <v>20</v>
@@ -13682,7 +13973,7 @@
         <v>0.570175438596491</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="60"/>
       <c r="C9" s="35" t="s">
         <v>46</v>
@@ -13715,7 +14006,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="61"/>
       <c r="C10" s="36" t="s">
         <v>49</v>
@@ -13748,7 +14039,7 @@
         <v>0.403100775193798</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="25.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" ht="25.8" x14ac:dyDescent="0.3">
       <c r="B11" s="44"/>
       <c r="C11" s="45"/>
       <c r="D11" s="18"/>
@@ -13761,7 +14052,7 @@
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
     </row>
-    <row r="12" spans="2:14" ht="25.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" ht="25.8" x14ac:dyDescent="0.3">
       <c r="B12" s="44"/>
       <c r="C12" s="45"/>
       <c r="D12" s="18"/>
@@ -13774,22 +14065,41 @@
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
     </row>
-    <row r="13" spans="2:14" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:12" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B13" s="44"/>
       <c r="C13" s="45"/>
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
-      <c r="H13" s="51" t="s">
-        <v>23</v>
-      </c>
+      <c r="H13" s="51"/>
       <c r="I13" s="52"/>
       <c r="J13" s="52"/>
       <c r="K13" s="52"/>
       <c r="L13" s="52"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="67" t="s">
+        <v>94</v>
+      </c>
       <c r="I14" s="1" t="s">
         <v>0</v>
       </c>
@@ -13802,11 +14112,24 @@
       <c r="L14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="69"/>
+      <c r="C15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="65">
+        <v>0.99491300000000005</v>
+      </c>
+      <c r="E15" s="65">
+        <v>0.97324100000000002</v>
+      </c>
+      <c r="F15" s="65">
+        <v>0.96469899999999997</v>
+      </c>
+      <c r="G15" s="66">
+        <v>0.98260899999999995</v>
+      </c>
       <c r="H15" s="1" t="s">
         <v>20</v>
       </c>
@@ -13823,7 +14146,23 @@
         <v>0.9913043478260869</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="69"/>
+      <c r="C16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16">
+        <v>0.99698600000000004</v>
+      </c>
+      <c r="E16">
+        <v>0.98484700000000003</v>
+      </c>
+      <c r="F16">
+        <v>0.97389999999999999</v>
+      </c>
+      <c r="G16">
+        <v>0.99636400000000003</v>
+      </c>
       <c r="H16" s="1" t="s">
         <v>46</v>
       </c>
@@ -13840,7 +14179,23 @@
         <v>0.99636400000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="70"/>
+      <c r="C17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17">
+        <v>0.996668</v>
+      </c>
+      <c r="E17">
+        <v>0.98686499999999999</v>
+      </c>
+      <c r="F17">
+        <v>0.98830300000000004</v>
+      </c>
+      <c r="G17">
+        <v>0.98603099999999999</v>
+      </c>
       <c r="H17" s="5" t="s">
         <v>49</v>
       </c>
@@ -13857,14 +14212,14 @@
         <v>0.97981499999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>72</v>
@@ -13882,7 +14237,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>71</v>
       </c>
@@ -13914,7 +14269,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>77</v>
       </c>
@@ -13950,7 +14305,7 @@
         <v>0.95300614189585864</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>78</v>
       </c>
@@ -13985,11 +14340,8 @@
       <c r="L22">
         <v>0.99342218759878964</v>
       </c>
-      <c r="N22" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>79</v>
       </c>
@@ -14022,7 +14374,22 @@
         <v>0.9917556338346204</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" t="s">
+        <v>83</v>
+      </c>
       <c r="H24" t="s">
         <v>58</v>
       </c>
@@ -14040,7 +14407,7 @@
         <v>0.9859496229056588</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B25" s="3"/>
       <c r="H25" t="s">
         <v>59</v>
@@ -14059,7 +14426,7 @@
         <v>0.9917760691866504</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H26" t="s">
         <v>60</v>
       </c>
@@ -14077,7 +14444,7 @@
         <v>0.99090863929910145</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H27" t="s">
         <v>61</v>
       </c>
@@ -14095,7 +14462,7 @@
         <v>0.92319830194643915</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H28" t="s">
         <v>62</v>
       </c>
@@ -14113,7 +14480,7 @@
         <v>0.99336754279004658</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H29" s="25" t="s">
         <v>63</v>
       </c>
@@ -14132,7 +14499,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="C2:G2"/>
@@ -14140,7 +14508,7 @@
     <mergeCell ref="H13:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added BLCA and Baselines
</commit_message>
<xml_diff>
--- a/summary/performances.xlsx
+++ b/summary/performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucan\OneDrive - Politecnico di Milano\PhD\progetti\CIBB2018\summary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="6_{451907C7-AB60-4BB7-A014-F4FB3421056D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{CCC14476-A39C-47FD-A318-50A911518322}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CC1F18-C3FE-449B-823B-C9B39D4D9524}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16236" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16236" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCGA_info" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="100">
   <si>
     <t>accuracy</t>
   </si>
@@ -329,6 +329,15 @@
   <si>
     <t>Baselines</t>
   </si>
+  <si>
+    <t>KNN</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>FFN</t>
+  </si>
 </sst>
 </file>
 
@@ -337,7 +346,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,6 +419,15 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -842,7 +860,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -934,6 +952,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -964,6 +990,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -988,20 +1023,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -7360,7 +7389,7 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="8" name="Gruppo 7">
+        <xdr:cNvPr id="12" name="Gruppo 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49471DEE-121C-431C-BE23-5F517047E699}"/>
@@ -7379,7 +7408,7 @@
       </xdr:grpSpPr>
       <xdr:graphicFrame macro="">
         <xdr:nvGraphicFramePr>
-          <xdr:cNvPr id="4" name="Grafico 3">
+          <xdr:cNvPr id="13" name="Grafico 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                 <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61D677F0-17E0-47BB-9320-9A1516CBD69D}"/>
@@ -7400,7 +7429,7 @@
       </xdr:graphicFrame>
       <xdr:graphicFrame macro="">
         <xdr:nvGraphicFramePr>
-          <xdr:cNvPr id="5" name="Grafico 4">
+          <xdr:cNvPr id="14" name="Grafico 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                 <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83C36CE6-D87F-421C-BAB9-68CC31E8D3D9}"/>
@@ -7423,7 +7452,7 @@
       </xdr:graphicFrame>
       <xdr:graphicFrame macro="">
         <xdr:nvGraphicFramePr>
-          <xdr:cNvPr id="6" name="Grafico 5">
+          <xdr:cNvPr id="15" name="Grafico 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                 <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D537FF2-207F-4888-AEFD-701D6C87F259}"/>
@@ -7446,7 +7475,7 @@
       </xdr:graphicFrame>
       <xdr:graphicFrame macro="">
         <xdr:nvGraphicFramePr>
-          <xdr:cNvPr id="7" name="Grafico 6">
+          <xdr:cNvPr id="16" name="Grafico 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                 <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{254ECF02-0E8F-4032-87E7-2B5E488AB6C0}"/>
@@ -7809,21 +7838,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF9BC486-AE94-4A41-83C2-002C0FB8F3B3}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView topLeftCell="A22" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -8550,30 +8579,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5BAE2A-9A59-4090-92C4-B579FFF4B317}">
-  <dimension ref="A1:F164"/>
+  <dimension ref="A1:M164"/>
   <sheetViews>
-    <sheetView topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="E140" sqref="E140"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33.6" x14ac:dyDescent="0.65">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:13" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A1" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>54</v>
       </c>
@@ -8589,8 +8625,23 @@
       <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I2" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -8610,8 +8661,23 @@
         <f>(C3*D3)/(2*D3-C3)</f>
         <v>0.93342783709138</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I3" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="50">
+        <v>0.991622</v>
+      </c>
+      <c r="K3" s="50">
+        <v>0.95774899999999996</v>
+      </c>
+      <c r="L3" s="50">
+        <v>0.92178400000000005</v>
+      </c>
+      <c r="M3" s="50">
+        <v>0.99826099999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -8631,8 +8697,23 @@
         <f t="shared" ref="F4:F67" si="0">(C4*D4)/(2*D4-C4)</f>
         <v>0.98142897589386802</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="50">
+        <v>0.99184899999999998</v>
+      </c>
+      <c r="K4" s="50">
+        <v>0.96051900000000001</v>
+      </c>
+      <c r="L4" s="50">
+        <v>0.925095</v>
+      </c>
+      <c r="M4" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -8652,8 +8733,23 @@
         <f t="shared" si="0"/>
         <v>0.99254105839416051</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="50">
+        <v>0.99686600000000003</v>
+      </c>
+      <c r="K5" s="50">
+        <v>0.98774200000000001</v>
+      </c>
+      <c r="L5" s="50">
+        <v>0.98369600000000001</v>
+      </c>
+      <c r="M5" s="50">
+        <v>0.99218499999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -8673,8 +8769,13 @@
         <f t="shared" si="0"/>
         <v>0.99254105839416051</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -8694,8 +8795,13 @@
         <f t="shared" si="0"/>
         <v>0.98743566479432654</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -8715,8 +8821,23 @@
         <f t="shared" si="0"/>
         <v>0.99254105839416051</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I8" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -8736,8 +8857,23 @@
         <f t="shared" si="0"/>
         <v>0.9381888723275893</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="50">
+        <v>0.98784300000000003</v>
+      </c>
+      <c r="K9" s="50">
+        <v>0.93200799999999995</v>
+      </c>
+      <c r="L9" s="50">
+        <v>0.96544799999999997</v>
+      </c>
+      <c r="M9" s="50">
+        <v>0.90308299999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -8757,8 +8893,23 @@
         <f t="shared" si="0"/>
         <v>0.97280700799135544</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="50">
+        <v>0.99256100000000003</v>
+      </c>
+      <c r="K10" s="50">
+        <v>0.960789</v>
+      </c>
+      <c r="L10" s="50">
+        <v>0.97269099999999997</v>
+      </c>
+      <c r="M10" s="50">
+        <v>0.950909</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="24" t="s">
         <v>16</v>
       </c>
@@ -8778,8 +8929,23 @@
         <f t="shared" si="0"/>
         <v>0.9381888723275893</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="50">
+        <v>0.99294300000000002</v>
+      </c>
+      <c r="K11" s="50">
+        <v>0.970947</v>
+      </c>
+      <c r="L11" s="50">
+        <v>0.99202000000000001</v>
+      </c>
+      <c r="M11" s="50">
+        <v>0.95206199999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
         <v>14</v>
       </c>
@@ -8799,8 +8965,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -8820,8 +8991,23 @@
         <f t="shared" si="0"/>
         <v>0.97963138493944213</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I13" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -8841,8 +9027,23 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="72">
+        <v>0.99491300000000005</v>
+      </c>
+      <c r="K14" s="72">
+        <v>0.97324100000000002</v>
+      </c>
+      <c r="L14" s="72">
+        <v>0.96469899999999997</v>
+      </c>
+      <c r="M14" s="73">
+        <v>0.98260899999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -8862,8 +9063,23 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="50">
+        <v>0.99698600000000004</v>
+      </c>
+      <c r="K15" s="50">
+        <v>0.98484700000000003</v>
+      </c>
+      <c r="L15" s="50">
+        <v>0.97389999999999999</v>
+      </c>
+      <c r="M15" s="50">
+        <v>0.99636400000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -8882,6 +9098,21 @@
       <c r="F16">
         <f t="shared" si="0"/>
         <v>0.98945470728207363</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" s="50">
+        <v>0.996668</v>
+      </c>
+      <c r="K16" s="50">
+        <v>0.98686499999999999</v>
+      </c>
+      <c r="L16" s="50">
+        <v>0.98830300000000004</v>
+      </c>
+      <c r="M16" s="50">
+        <v>0.98603099999999999</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -12004,10 +12235,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W34"/>
+  <dimension ref="A1:X34"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" activeCellId="2" sqref="A19:XFD19 A11:XFD11 A6:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12022,30 +12253,30 @@
     <col min="11" max="19" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:24" s="2" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A1" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="G1" s="51" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="G1" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="M1" s="51" t="s">
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="M1" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -12082,15 +12313,15 @@
       <c r="Q2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="53" t="s">
+      <c r="S2" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
+      <c r="V2" s="57"/>
+      <c r="W2" s="57"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -12137,7 +12368,7 @@
         <v>0.8727243452125375</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -12184,7 +12415,7 @@
         <v>0.94075163398692807</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -12231,7 +12462,7 @@
         <v>0.92877816627816634</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
         <v>7</v>
       </c>
@@ -12278,7 +12509,7 @@
         <v>0.93029331779331792</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -12325,7 +12556,7 @@
         <v>0.92328224377020118</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -12372,7 +12603,7 @@
         <v>0.90674048174048172</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -12418,8 +12649,23 @@
       <c r="Q9">
         <v>0.92949640287769797</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="T9" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -12465,8 +12711,23 @@
       <c r="Q10">
         <v>0.92057008192122092</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="T10" s="75" t="s">
+        <v>98</v>
+      </c>
+      <c r="U10" s="8">
+        <v>0.98966799999999999</v>
+      </c>
+      <c r="V10" s="8">
+        <v>0.897123</v>
+      </c>
+      <c r="W10" s="8">
+        <v>0.87152399999999997</v>
+      </c>
+      <c r="X10" s="8">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="33" t="s">
         <v>12</v>
       </c>
@@ -12512,8 +12773,23 @@
       <c r="Q11">
         <v>0.95059434621915884</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="T11" s="75" t="s">
+        <v>99</v>
+      </c>
+      <c r="U11" s="8">
+        <v>0.99106899999999998</v>
+      </c>
+      <c r="V11" s="8">
+        <v>0.87263500000000005</v>
+      </c>
+      <c r="W11" s="8">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="X11" s="8">
+        <v>0.85666699999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -12560,7 +12836,7 @@
         <v>0.93925925925925924</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -12607,7 +12883,7 @@
         <v>0.93595744680851067</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -12654,7 +12930,7 @@
         <v>0.93129770992366423</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -12701,7 +12977,7 @@
         <v>0.96538314176245199</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -12999,13 +13275,13 @@
       <c r="K22">
         <v>0.97981499999999999</v>
       </c>
-      <c r="M22" s="54" t="s">
+      <c r="M22" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="N22" s="55"/>
-      <c r="O22" s="55"/>
-      <c r="P22" s="55"/>
-      <c r="Q22" s="55"/>
+      <c r="N22" s="59"/>
+      <c r="O22" s="59"/>
+      <c r="P22" s="59"/>
+      <c r="Q22" s="59"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
@@ -13331,13 +13607,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="33.6" x14ac:dyDescent="0.65">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -13369,13 +13645,13 @@
       <c r="E3">
         <v>0.97312299999999996</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -13421,13 +13697,13 @@
       <c r="A8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="33.6" x14ac:dyDescent="0.65">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
@@ -13551,21 +13827,21 @@
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="2:13" s="3" customFormat="1" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
       <c r="G1" s="22"/>
-      <c r="I1" s="51" t="s">
+      <c r="I1" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
     </row>
     <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="10"/>
@@ -13708,11 +13984,11 @@
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="56"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C15" s="20"/>
@@ -13734,8 +14010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0D92E8-BE8B-7042-85EF-6FE2473B88F2}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="C10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13756,23 +14032,23 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="62" t="s">
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="64"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="71"/>
     </row>
     <row r="3" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="64" t="s">
         <v>86</v>
       </c>
       <c r="C3" s="43" t="s">
@@ -13807,7 +14083,7 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="58"/>
+      <c r="B4" s="65"/>
       <c r="C4" s="35" t="s">
         <v>20</v>
       </c>
@@ -13840,7 +14116,7 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="58"/>
+      <c r="B5" s="65"/>
       <c r="C5" s="35" t="s">
         <v>46</v>
       </c>
@@ -13873,7 +14149,7 @@
       </c>
     </row>
     <row r="6" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="58"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="36" t="s">
         <v>49</v>
       </c>
@@ -13906,7 +14182,7 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="66" t="s">
         <v>87</v>
       </c>
       <c r="C7" s="38" t="s">
@@ -13941,7 +14217,7 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="60"/>
+      <c r="B8" s="67"/>
       <c r="C8" s="35" t="s">
         <v>20</v>
       </c>
@@ -13974,7 +14250,7 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="60"/>
+      <c r="B9" s="67"/>
       <c r="C9" s="35" t="s">
         <v>46</v>
       </c>
@@ -14007,7 +14283,7 @@
       </c>
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="61"/>
+      <c r="B10" s="68"/>
       <c r="C10" s="36" t="s">
         <v>49</v>
       </c>
@@ -14072,17 +14348,17 @@
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="52"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="56"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="68" t="s">
+      <c r="B14" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="67" t="s">
+      <c r="C14" s="49" t="s">
         <v>95</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -14097,7 +14373,7 @@
       <c r="G14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H14" s="67" t="s">
+      <c r="H14" s="49" t="s">
         <v>94</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -14114,40 +14390,40 @@
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="69"/>
+      <c r="B15" s="62"/>
       <c r="C15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="65">
+      <c r="D15" s="47">
         <v>0.99491300000000005</v>
       </c>
-      <c r="E15" s="65">
+      <c r="E15" s="47">
         <v>0.97324100000000002</v>
       </c>
-      <c r="F15" s="65">
+      <c r="F15" s="47">
         <v>0.96469899999999997</v>
       </c>
-      <c r="G15" s="66">
+      <c r="G15" s="48">
         <v>0.98260899999999995</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="34">
+      <c r="I15" s="47">
         <v>0.98851104186424599</v>
       </c>
-      <c r="J15" s="34">
+      <c r="J15" s="47">
         <v>0.94562199235649746</v>
       </c>
-      <c r="K15" s="34">
+      <c r="K15" s="47">
         <v>0.91041666666666676</v>
       </c>
-      <c r="L15" s="34">
+      <c r="L15" s="47">
         <v>0.9913043478260869</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="69"/>
+      <c r="B16" s="62"/>
       <c r="C16" s="1" t="s">
         <v>46</v>
       </c>
@@ -14180,7 +14456,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="70"/>
+      <c r="B17" s="63"/>
       <c r="C17" s="5" t="s">
         <v>49</v>
       </c>

</xml_diff>